<commit_message>
added designs for led light bar and valve control boards;  updated parts list to include aalborg components
</commit_message>
<xml_diff>
--- a/Materials List/LADY GAGA V2 Materials.xlsx
+++ b/Materials List/LADY GAGA V2 Materials.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="220">
   <si>
     <t>Description</t>
   </si>
@@ -561,9 +561,6 @@
     <t>valve controller board</t>
   </si>
   <si>
-    <t>schematic and parts list forthcoming</t>
-  </si>
-  <si>
     <t>led light bars</t>
   </si>
   <si>
@@ -576,9 +573,6 @@
     <t>779051-01</t>
   </si>
   <si>
-    <t>Other Stuff</t>
-  </si>
-  <si>
     <t>12V computer power supply</t>
   </si>
   <si>
@@ -646,6 +640,42 @@
   </si>
   <si>
     <t>teflon fep tubing, black 0.020"  ID x 1/16" OD</t>
+  </si>
+  <si>
+    <t>Aalborg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GFC17A-VADL2-C0A </t>
+  </si>
+  <si>
+    <t>gas flow controller; aluminum housing; viton seals</t>
+  </si>
+  <si>
+    <t>calibrated for air 5L/min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3AB-09-SS </t>
+  </si>
+  <si>
+    <t>calibrated for air 100mL/min</t>
+  </si>
+  <si>
+    <t>3AB-04-SS</t>
+  </si>
+  <si>
+    <t>P11A3-TA0A</t>
+  </si>
+  <si>
+    <t>flow meter - housing</t>
+  </si>
+  <si>
+    <t>flow meter - flow tube 0-10 L/min direct reading</t>
+  </si>
+  <si>
+    <t>102-16-CA-TN</t>
+  </si>
+  <si>
+    <t>separate pcb and parts list</t>
   </si>
 </sst>
 </file>
@@ -1029,10 +1059,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G132"/>
+  <dimension ref="A1:G141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="C119" sqref="C119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1740,7 +1770,7 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B37">
         <v>1519</v>
@@ -3125,10 +3155,10 @@
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
+        <v>188</v>
+      </c>
+      <c r="B101" s="6" t="s">
         <v>190</v>
-      </c>
-      <c r="B101" s="6" t="s">
-        <v>192</v>
       </c>
       <c r="C101">
         <v>4.99</v>
@@ -3150,10 +3180,10 @@
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
+        <v>189</v>
+      </c>
+      <c r="B102" s="6" t="s">
         <v>191</v>
-      </c>
-      <c r="B102" s="6" t="s">
-        <v>193</v>
       </c>
       <c r="C102">
         <v>5.01</v>
@@ -3175,10 +3205,10 @@
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B103" s="6" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C103">
         <v>5.65</v>
@@ -3200,10 +3230,10 @@
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B104" s="6" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C104">
         <v>7.08</v>
@@ -3225,10 +3255,10 @@
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B105" s="6" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C105">
         <v>2.87</v>
@@ -3250,10 +3280,10 @@
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B106" s="6" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C106">
         <v>3.13</v>
@@ -3275,10 +3305,10 @@
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B107" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C107">
         <v>13.94</v>
@@ -3300,7 +3330,7 @@
     </row>
     <row r="109" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A109" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
@@ -3328,10 +3358,10 @@
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B111" s="7" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C111">
         <v>381.45</v>
@@ -3354,7 +3384,7 @@
     </row>
     <row r="113" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A113" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
@@ -3382,10 +3412,10 @@
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="B115" t="s">
         <v>184</v>
-      </c>
-      <c r="B115" t="s">
-        <v>185</v>
       </c>
       <c r="C115" s="5">
         <v>169</v>
@@ -3433,59 +3463,217 @@
         <v>180</v>
       </c>
       <c r="B120" t="s">
-        <v>181</v>
+        <v>219</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B121" t="s">
-        <v>181</v>
+        <v>219</v>
       </c>
     </row>
     <row r="123" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A123" s="2" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A124" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D124" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E124" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F124" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G124" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A125" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="B125" t="s">
+        <v>209</v>
+      </c>
+      <c r="C125" s="5">
+        <v>852</v>
+      </c>
+      <c r="D125" s="5">
+        <v>3</v>
+      </c>
+      <c r="E125" s="5">
+        <v>0</v>
+      </c>
+      <c r="F125">
+        <f>(D125+E125)</f>
+        <v>3</v>
+      </c>
+      <c r="G125">
+        <f t="shared" ref="G125" si="14">(C125*F125)</f>
+        <v>2556</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A126" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="B126" t="s">
+        <v>212</v>
+      </c>
+      <c r="C126" s="5"/>
+      <c r="D126" s="5">
+        <v>1</v>
+      </c>
+      <c r="E126" s="5">
+        <v>0</v>
+      </c>
+      <c r="F126">
+        <f t="shared" ref="F126:F128" si="15">(D126+E126)</f>
+        <v>1</v>
+      </c>
+      <c r="G126">
+        <f t="shared" ref="G126:G128" si="16">(C126*F126)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A127" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="B127" t="s">
+        <v>214</v>
+      </c>
+      <c r="C127" s="5"/>
+      <c r="D127" s="5">
+        <v>2</v>
+      </c>
+      <c r="E127" s="5">
+        <v>0</v>
+      </c>
+      <c r="F127">
+        <f t="shared" si="15"/>
+        <v>2</v>
+      </c>
+      <c r="G127">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A128" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="B128" t="s">
+        <v>215</v>
+      </c>
+      <c r="C128" s="5">
+        <v>277</v>
+      </c>
+      <c r="D128" s="5">
+        <v>1</v>
+      </c>
+      <c r="E128" s="5">
+        <v>0</v>
+      </c>
+      <c r="F128">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
+      <c r="G128">
+        <f t="shared" si="16"/>
+        <v>277</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A129" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="B129" t="s">
+        <v>218</v>
+      </c>
+      <c r="C129" s="5"/>
+      <c r="D129" s="5">
+        <v>1</v>
+      </c>
+      <c r="E129" s="5"/>
+      <c r="F129">
+        <f t="shared" ref="F129" si="17">(D129+E129)</f>
+        <v>1</v>
+      </c>
+      <c r="G129">
+        <f t="shared" ref="G129" si="18">(C129*F129)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A130" s="5"/>
+      <c r="C130" s="5"/>
+      <c r="D130" s="5"/>
+      <c r="E130" s="5"/>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A131" s="5"/>
+      <c r="C131" s="5"/>
+      <c r="D131" s="5"/>
+      <c r="E131" s="5"/>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A132" s="5"/>
+      <c r="C132" s="5"/>
+      <c r="D132" s="5"/>
+      <c r="E132" s="5"/>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A127" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A129" t="s">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A130" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A131" t="s">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A132" t="s">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
         <v>178</v>
       </c>
     </row>

</xml_diff>

<commit_message>
created 80-20 enclosure; added bill of materials to materials list and enclosure to parts list
</commit_message>
<xml_diff>
--- a/Materials List/LADY GAGA V2 Materials.xlsx
+++ b/Materials List/LADY GAGA V2 Materials.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="222">
   <si>
     <t>Description</t>
   </si>
@@ -639,9 +639,6 @@
     <t>hinged clamp for pneumatic compression</t>
   </si>
   <si>
-    <t>teflon fep tubing, black 0.020"  ID x 1/16" OD</t>
-  </si>
-  <si>
     <t>Aalborg</t>
   </si>
   <si>
@@ -676,6 +673,15 @@
   </si>
   <si>
     <t>separate pcb and parts list</t>
+  </si>
+  <si>
+    <t>teflon fep tubing, natural 0.030"  ID x 1/16" OD</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1520L</t>
+  </si>
+  <si>
+    <t>enclosure</t>
   </si>
 </sst>
 </file>
@@ -1059,10 +1065,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G141"/>
+  <dimension ref="A1:G142"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="C119" sqref="C119"/>
+      <selection activeCell="I114" sqref="I114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1704,18 +1710,18 @@
         <v>46.82</v>
       </c>
       <c r="D34">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E34">
         <v>2</v>
       </c>
       <c r="F34">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="G34">
         <f t="shared" si="1"/>
-        <v>842.76</v>
+        <v>1030.04</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -1770,13 +1776,13 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>207</v>
-      </c>
-      <c r="B37">
-        <v>1519</v>
+        <v>219</v>
+      </c>
+      <c r="B37" t="s">
+        <v>220</v>
       </c>
       <c r="C37">
-        <v>37.49</v>
+        <v>85</v>
       </c>
       <c r="D37">
         <v>1</v>
@@ -1790,7 +1796,7 @@
       </c>
       <c r="G37">
         <f t="shared" ref="G37" si="3">(C37*F37)</f>
-        <v>37.49</v>
+        <v>85</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -1801,7 +1807,7 @@
         <v>1534</v>
       </c>
       <c r="C38">
-        <v>33.61</v>
+        <v>85.19</v>
       </c>
       <c r="D38">
         <v>1</v>
@@ -1815,7 +1821,7 @@
       </c>
       <c r="G38">
         <f t="shared" si="1"/>
-        <v>33.61</v>
+        <v>85.19</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -2303,18 +2309,18 @@
         <v>18.16</v>
       </c>
       <c r="D61">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E61">
         <v>4</v>
       </c>
       <c r="F61">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G61">
         <f t="shared" si="1"/>
-        <v>72.64</v>
+        <v>145.28</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
@@ -3380,69 +3386,83 @@
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B112" s="6"/>
-    </row>
-    <row r="113" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A113" s="2" t="s">
+      <c r="A112" t="s">
+        <v>221</v>
+      </c>
+      <c r="B112" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="C112">
+        <v>1702.97</v>
+      </c>
+      <c r="D112">
+        <v>1</v>
+      </c>
+      <c r="E112">
+        <v>0</v>
+      </c>
+      <c r="F112">
+        <v>1</v>
+      </c>
+      <c r="G112">
+        <v>1702.97</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B113" s="6"/>
+    </row>
+    <row r="114" spans="1:7" ht="21" x14ac:dyDescent="0.35">
+      <c r="A114" s="2" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A114" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B114" s="1" t="s">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A115" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B115" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C114" s="1" t="s">
+      <c r="C115" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D114" s="1" t="s">
+      <c r="D115" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E114" s="1" t="s">
+      <c r="E115" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F114" s="1" t="s">
+      <c r="F115" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G114" s="1" t="s">
+      <c r="G115" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A115" s="5" t="s">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A116" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="B115" t="s">
+      <c r="B116" t="s">
         <v>184</v>
       </c>
-      <c r="C115" s="5">
+      <c r="C116" s="5">
         <v>169</v>
       </c>
-      <c r="D115" s="5">
+      <c r="D116" s="5">
         <v>2</v>
       </c>
-      <c r="E115" s="5">
-        <v>0</v>
-      </c>
-      <c r="F115">
-        <f t="shared" ref="F115" si="12">(D115+E115)</f>
+      <c r="E116" s="5">
+        <v>0</v>
+      </c>
+      <c r="F116">
+        <f t="shared" ref="F116" si="12">(D116+E116)</f>
         <v>2</v>
       </c>
-      <c r="G115">
-        <f t="shared" ref="G115" si="13">(C115*F115)</f>
+      <c r="G116">
+        <f t="shared" ref="G116" si="13">(C116*F116)</f>
         <v>338</v>
       </c>
-    </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A116" s="1"/>
-      <c r="B116" s="1"/>
-      <c r="C116" s="1"/>
-      <c r="D116" s="1"/>
-      <c r="E116" s="1"/>
-      <c r="F116" s="1"/>
-      <c r="G116" s="1"/>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" s="1"/>
@@ -3453,177 +3473,180 @@
       <c r="F117" s="1"/>
       <c r="G117" s="1"/>
     </row>
-    <row r="118" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A118" s="2" t="s">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A118" s="1"/>
+      <c r="B118" s="1"/>
+      <c r="C118" s="1"/>
+      <c r="D118" s="1"/>
+      <c r="E118" s="1"/>
+      <c r="F118" s="1"/>
+      <c r="G118" s="1"/>
+    </row>
+    <row r="119" spans="1:7" ht="21" x14ac:dyDescent="0.35">
+      <c r="A119" s="2" t="s">
         <v>179</v>
-      </c>
-    </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
-        <v>180</v>
-      </c>
-      <c r="B120" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
+        <v>180</v>
+      </c>
+      <c r="B121" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
         <v>181</v>
       </c>
-      <c r="B121" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="123" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A123" s="2" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A124" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B124" s="1" t="s">
+      <c r="B122" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" ht="21" x14ac:dyDescent="0.35">
+      <c r="A124" s="2" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A125" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B125" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C124" s="1" t="s">
+      <c r="C125" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D124" s="1" t="s">
+      <c r="D125" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E124" s="1" t="s">
+      <c r="E125" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F124" s="1" t="s">
+      <c r="F125" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G124" s="1" t="s">
+      <c r="G125" s="1" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A125" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="B125" t="s">
-        <v>209</v>
-      </c>
-      <c r="C125" s="5">
-        <v>852</v>
-      </c>
-      <c r="D125" s="5">
-        <v>3</v>
-      </c>
-      <c r="E125" s="5">
-        <v>0</v>
-      </c>
-      <c r="F125">
-        <f>(D125+E125)</f>
-        <v>3</v>
-      </c>
-      <c r="G125">
-        <f t="shared" ref="G125" si="14">(C125*F125)</f>
-        <v>2556</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" s="5" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B126" t="s">
-        <v>212</v>
-      </c>
-      <c r="C126" s="5"/>
+        <v>208</v>
+      </c>
+      <c r="C126" s="5">
+        <v>852</v>
+      </c>
       <c r="D126" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E126" s="5">
         <v>0</v>
       </c>
       <c r="F126">
-        <f t="shared" ref="F126:F128" si="15">(D126+E126)</f>
-        <v>1</v>
+        <f>(D126+E126)</f>
+        <v>3</v>
       </c>
       <c r="G126">
-        <f t="shared" ref="G126:G128" si="16">(C126*F126)</f>
-        <v>0</v>
+        <f t="shared" ref="G126" si="14">(C126*F126)</f>
+        <v>2556</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" s="5" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B127" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C127" s="5"/>
       <c r="D127" s="5">
+        <v>1</v>
+      </c>
+      <c r="E127" s="5">
+        <v>0</v>
+      </c>
+      <c r="F127">
+        <f t="shared" ref="F127:F129" si="15">(D127+E127)</f>
+        <v>1</v>
+      </c>
+      <c r="G127">
+        <f t="shared" ref="G127:G129" si="16">(C127*F127)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A128" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="B128" t="s">
+        <v>213</v>
+      </c>
+      <c r="C128" s="5"/>
+      <c r="D128" s="5">
         <v>2</v>
       </c>
-      <c r="E127" s="5">
-        <v>0</v>
-      </c>
-      <c r="F127">
+      <c r="E128" s="5">
+        <v>0</v>
+      </c>
+      <c r="F128">
         <f t="shared" si="15"/>
         <v>2</v>
       </c>
-      <c r="G127">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A128" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="B128" t="s">
-        <v>215</v>
-      </c>
-      <c r="C128" s="5">
-        <v>277</v>
-      </c>
-      <c r="D128" s="5">
-        <v>1</v>
-      </c>
-      <c r="E128" s="5">
-        <v>0</v>
-      </c>
-      <c r="F128">
-        <f t="shared" si="15"/>
-        <v>1</v>
-      </c>
       <c r="G128">
         <f t="shared" si="16"/>
-        <v>277</v>
+        <v>0</v>
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="B129" t="s">
+        <v>214</v>
+      </c>
+      <c r="C129" s="5">
+        <v>277</v>
+      </c>
+      <c r="D129" s="5">
+        <v>1</v>
+      </c>
+      <c r="E129" s="5">
+        <v>0</v>
+      </c>
+      <c r="F129">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
+      <c r="G129">
+        <f t="shared" si="16"/>
+        <v>277</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A130" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="B130" t="s">
         <v>217</v>
       </c>
-      <c r="B129" t="s">
-        <v>218</v>
-      </c>
-      <c r="C129" s="5"/>
-      <c r="D129" s="5">
-        <v>1</v>
-      </c>
-      <c r="E129" s="5"/>
-      <c r="F129">
-        <f t="shared" ref="F129" si="17">(D129+E129)</f>
-        <v>1</v>
-      </c>
-      <c r="G129">
-        <f t="shared" ref="G129" si="18">(C129*F129)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A130" s="5"/>
       <c r="C130" s="5"/>
-      <c r="D130" s="5"/>
+      <c r="D130" s="5">
+        <v>1</v>
+      </c>
       <c r="E130" s="5"/>
+      <c r="F130">
+        <f t="shared" ref="F130" si="17">(D130+E130)</f>
+        <v>1</v>
+      </c>
+      <c r="G130">
+        <f t="shared" ref="G130" si="18">(C130*F130)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" s="5"/>
@@ -3638,42 +3661,48 @@
       <c r="E132" s="5"/>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
-        <v>185</v>
-      </c>
+      <c r="A133" s="5"/>
+      <c r="C133" s="5"/>
+      <c r="D133" s="5"/>
+      <c r="E133" s="5"/>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
         <v>192</v>
-      </c>
-    </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>203</v>
+        <v>176</v>
       </c>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>177</v>
+        <v>203</v>
       </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
         <v>178</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added plans for measuring gradient; updated bill of materials to reflect these plans; added some documentation about connections
</commit_message>
<xml_diff>
--- a/Materials List/LADY GAGA V2 Materials.xlsx
+++ b/Materials List/LADY GAGA V2 Materials.xlsx
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="246">
   <si>
     <t>Description</t>
   </si>
@@ -682,6 +682,78 @@
   </si>
   <si>
     <t>enclosure</t>
+  </si>
+  <si>
+    <t>Top Plate for Gradient measurement</t>
+  </si>
+  <si>
+    <t>top plate for gradient measurement</t>
+  </si>
+  <si>
+    <t>Clamp for Pidtech plus</t>
+  </si>
+  <si>
+    <t>simple clamp block for pidtech plus</t>
+  </si>
+  <si>
+    <t>flow block for draw sampling</t>
+  </si>
+  <si>
+    <t>flow block for measuring concentration in a stream</t>
+  </si>
+  <si>
+    <t>Aluminum (anodization optional)</t>
+  </si>
+  <si>
+    <t>Aluminum  (anodization optional) or stainless</t>
+  </si>
+  <si>
+    <t>Aluminum  (anodization optional)</t>
+  </si>
+  <si>
+    <t>Baseline-Mocon</t>
+  </si>
+  <si>
+    <t>ZPP6018001 042-208</t>
+  </si>
+  <si>
+    <t>Pidtech Plus Black (0.05 to 2000 ppm)</t>
+  </si>
+  <si>
+    <t>Pidtech Plus Silver (&lt;5ppb to 20 ppm)</t>
+  </si>
+  <si>
+    <t>ZPP6018002 042-209</t>
+  </si>
+  <si>
+    <t>1/4" tube fitting to 1/8" NPT M, stainless</t>
+  </si>
+  <si>
+    <t>SS-400-1-2</t>
+  </si>
+  <si>
+    <t>SS-200-1-2</t>
+  </si>
+  <si>
+    <t>1/8" tube fitting to 1/8" NPT M, stainless</t>
+  </si>
+  <si>
+    <t>get latest version</t>
+  </si>
+  <si>
+    <t>NOTE: part numbers may have changed / new version available</t>
+  </si>
+  <si>
+    <t>EPDM O-Ring AS568A Dash Number 210</t>
+  </si>
+  <si>
+    <t>9557K478</t>
+  </si>
+  <si>
+    <t>EPDM O-Ring AS568A Dash Number 211</t>
+  </si>
+  <si>
+    <t>9557K479</t>
   </si>
 </sst>
 </file>
@@ -1065,10 +1137,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G142"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:H154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="I114" sqref="I114"/>
+    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
+      <selection activeCell="H106" sqref="H106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1078,6 +1151,7 @@
     <col min="3" max="3" width="25" customWidth="1"/>
     <col min="4" max="4" width="14.7109375" customWidth="1"/>
     <col min="7" max="7" width="26.42578125" customWidth="1"/>
+    <col min="8" max="8" width="30.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.35">
@@ -1146,7 +1220,7 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <f t="shared" ref="F4:F62" si="0">(D4+E4)</f>
+        <f t="shared" ref="F4:F65" si="0">(D4+E4)</f>
         <v>1</v>
       </c>
       <c r="G4" t="s">
@@ -1333,1169 +1407,1157 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A14" s="2" t="s">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>222</v>
+      </c>
+      <c r="B13" t="s">
+        <v>223</v>
+      </c>
+      <c r="C13" t="s">
+        <v>228</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>224</v>
+      </c>
+      <c r="B14" t="s">
+        <v>225</v>
+      </c>
+      <c r="C14" t="s">
+        <v>229</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>226</v>
+      </c>
+      <c r="B15" t="s">
+        <v>227</v>
+      </c>
+      <c r="C15" t="s">
+        <v>230</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="21" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B15" s="1" t="s">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="F18" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="G18" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>41</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B19" t="s">
         <v>42</v>
       </c>
-      <c r="C16">
+      <c r="C19">
         <v>690</v>
       </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-      <c r="F16">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="G16">
-        <f>(C16*F16)</f>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <f>(C19*F19)</f>
         <v>690</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>44</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B20" t="s">
         <v>43</v>
       </c>
-      <c r="C17">
+      <c r="C20">
         <v>4.74</v>
       </c>
-      <c r="D17">
+      <c r="D20">
         <v>5</v>
       </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
-      <c r="F17">
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G17">
-        <f t="shared" ref="G17:G62" si="1">(C17*F17)</f>
+      <c r="G20">
+        <f t="shared" ref="G20:G65" si="1">(C20*F20)</f>
         <v>23.700000000000003</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>45</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B21" t="s">
         <v>46</v>
       </c>
-      <c r="C18">
+      <c r="C21">
         <v>4.74</v>
       </c>
-      <c r="D18">
+      <c r="D21">
         <v>2</v>
       </c>
-      <c r="E18">
-        <v>1</v>
-      </c>
-      <c r="F18">
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="G18">
+      <c r="G21">
         <f t="shared" si="1"/>
         <v>14.22</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>47</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B22" t="s">
         <v>48</v>
       </c>
-      <c r="C19">
+      <c r="C22">
         <v>4.97</v>
       </c>
-      <c r="D19">
+      <c r="D22">
         <v>3</v>
       </c>
-      <c r="E19">
-        <v>0</v>
-      </c>
-      <c r="F19">
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="G19">
+      <c r="G22">
         <f t="shared" si="1"/>
         <v>14.91</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>49</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B23" t="s">
         <v>50</v>
       </c>
-      <c r="C20">
+      <c r="C23">
         <v>7.03</v>
       </c>
-      <c r="D20">
+      <c r="D23">
         <v>5</v>
       </c>
-      <c r="E20">
-        <v>0</v>
-      </c>
-      <c r="F20">
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G20">
+      <c r="G23">
         <f t="shared" si="1"/>
         <v>35.15</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>51</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B24" t="s">
         <v>52</v>
       </c>
-      <c r="C21">
+      <c r="C24">
         <v>9.1</v>
       </c>
-      <c r="D21">
+      <c r="D24">
         <v>15</v>
       </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
-      <c r="F21">
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="G21">
+      <c r="G24">
         <f t="shared" si="1"/>
         <v>136.5</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>53</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B25" t="s">
         <v>54</v>
       </c>
-      <c r="C22">
+      <c r="C25">
         <v>8.75</v>
       </c>
-      <c r="D22">
+      <c r="D25">
         <v>15</v>
       </c>
-      <c r="E22">
-        <v>0</v>
-      </c>
-      <c r="F22">
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="G22">
+      <c r="G25">
         <f t="shared" si="1"/>
         <v>131.25</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>55</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B26" t="s">
         <v>56</v>
       </c>
-      <c r="C23">
+      <c r="C26">
         <v>23</v>
       </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-      <c r="E23">
-        <v>1</v>
-      </c>
-      <c r="F23">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="G23">
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G26">
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>57</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B27" t="s">
         <v>58</v>
       </c>
-      <c r="C24">
+      <c r="C27">
         <v>11.3</v>
       </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
-      <c r="E24">
-        <v>1</v>
-      </c>
-      <c r="F24">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="G24">
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G27">
         <f t="shared" si="1"/>
         <v>11.3</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>59</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B28" t="s">
         <v>60</v>
       </c>
-      <c r="C25">
+      <c r="C28">
         <v>106.1</v>
       </c>
-      <c r="D25">
-        <v>0</v>
-      </c>
-      <c r="E25">
-        <v>1</v>
-      </c>
-      <c r="F25">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="G25">
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G28">
         <f t="shared" si="1"/>
         <v>106.1</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>61</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B29" t="s">
         <v>62</v>
       </c>
-      <c r="C26">
+      <c r="C29">
         <v>82</v>
       </c>
-      <c r="D26">
+      <c r="D29">
         <v>2</v>
       </c>
-      <c r="E26">
-        <v>0</v>
-      </c>
-      <c r="F26">
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G26">
+      <c r="G29">
         <f t="shared" si="1"/>
         <v>164</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>63</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B30" t="s">
         <v>64</v>
       </c>
-      <c r="C27">
+      <c r="C30">
         <v>34</v>
       </c>
-      <c r="D27">
+      <c r="D30">
         <v>2</v>
       </c>
-      <c r="E27">
-        <v>0</v>
-      </c>
-      <c r="F27">
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G27">
+      <c r="G30">
         <f t="shared" si="1"/>
         <v>68</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A32" s="2" t="s">
+    <row r="35" spans="1:7" ht="21" x14ac:dyDescent="0.35">
+      <c r="A35" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B33" s="1" t="s">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C36" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="D36" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="E36" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F33" s="1" t="s">
+      <c r="F36" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G33" s="1" t="s">
+      <c r="G36" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>68</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B37" t="s">
         <v>69</v>
       </c>
-      <c r="C34">
+      <c r="C37">
         <v>46.82</v>
       </c>
-      <c r="D34">
+      <c r="D37">
         <v>20</v>
       </c>
-      <c r="E34">
+      <c r="E37">
         <v>2</v>
       </c>
-      <c r="F34">
+      <c r="F37">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="G34">
+      <c r="G37">
         <f t="shared" si="1"/>
         <v>1030.04</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>70</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B38" t="s">
         <v>71</v>
       </c>
-      <c r="C35">
+      <c r="C38">
         <v>46.76</v>
       </c>
-      <c r="D35">
-        <v>0</v>
-      </c>
-      <c r="E35">
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="E38">
         <v>4</v>
       </c>
-      <c r="F35">
+      <c r="F38">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="G35">
+      <c r="G38">
         <f t="shared" si="1"/>
         <v>187.04</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>72</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B39" t="s">
         <v>73</v>
       </c>
-      <c r="C36">
+      <c r="C39">
         <v>96.48</v>
       </c>
-      <c r="D36">
-        <v>1</v>
-      </c>
-      <c r="E36">
-        <v>0</v>
-      </c>
-      <c r="F36">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="G36">
+      <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G39">
         <f t="shared" si="1"/>
         <v>96.48</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>219</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B40" t="s">
         <v>220</v>
       </c>
-      <c r="C37">
+      <c r="C40">
         <v>85</v>
       </c>
-      <c r="D37">
-        <v>1</v>
-      </c>
-      <c r="E37">
-        <v>0</v>
-      </c>
-      <c r="F37">
-        <f t="shared" ref="F37" si="2">(D37+E37)</f>
-        <v>1</v>
-      </c>
-      <c r="G37">
-        <f t="shared" ref="G37" si="3">(C37*F37)</f>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40">
+        <f t="shared" ref="F40" si="2">(D40+E40)</f>
+        <v>1</v>
+      </c>
+      <c r="G40">
+        <f t="shared" ref="G40" si="3">(C40*F40)</f>
         <v>85</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>74</v>
       </c>
-      <c r="B38">
+      <c r="B41">
         <v>1534</v>
       </c>
-      <c r="C38">
+      <c r="C41">
         <v>85.19</v>
       </c>
-      <c r="D38">
-        <v>1</v>
-      </c>
-      <c r="E38">
-        <v>0</v>
-      </c>
-      <c r="F38">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="G38">
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G41">
         <f t="shared" si="1"/>
         <v>85.19</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B42" t="s">
         <v>76</v>
       </c>
-      <c r="C39">
+      <c r="C42">
         <v>11.91</v>
       </c>
-      <c r="D39">
-        <v>1</v>
-      </c>
-      <c r="E39">
-        <v>1</v>
-      </c>
-      <c r="F39">
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42">
+        <v>1</v>
+      </c>
+      <c r="F42">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G39">
+      <c r="G42">
         <f t="shared" si="1"/>
         <v>23.82</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>77</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B43" t="s">
         <v>78</v>
       </c>
-      <c r="C40">
+      <c r="C43">
         <v>11.91</v>
       </c>
-      <c r="D40">
-        <v>1</v>
-      </c>
-      <c r="E40">
-        <v>0</v>
-      </c>
-      <c r="F40">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="G40">
+      <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G43">
         <f t="shared" si="1"/>
         <v>11.91</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>79</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B44" t="s">
         <v>80</v>
       </c>
-      <c r="C41">
+      <c r="C44">
         <v>85.36</v>
       </c>
-      <c r="D41">
+      <c r="D44">
         <v>2</v>
       </c>
-      <c r="E41">
-        <v>0</v>
-      </c>
-      <c r="F41">
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="F44">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G41">
+      <c r="G44">
         <f t="shared" si="1"/>
         <v>170.72</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>81</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B45" t="s">
         <v>82</v>
       </c>
-      <c r="C42">
+      <c r="C45">
         <v>6.65</v>
       </c>
-      <c r="D42">
-        <v>0</v>
-      </c>
-      <c r="E42">
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45">
         <v>2</v>
       </c>
-      <c r="F42">
+      <c r="F45">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G42">
+      <c r="G45">
         <f t="shared" si="1"/>
         <v>13.3</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>83</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B46" t="s">
         <v>84</v>
       </c>
-      <c r="C43">
+      <c r="C46">
         <v>10.55</v>
       </c>
-      <c r="D43">
-        <v>1</v>
-      </c>
-      <c r="E43">
-        <v>1</v>
-      </c>
-      <c r="F43">
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46">
+        <v>1</v>
+      </c>
+      <c r="F46">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G43">
+      <c r="G46">
         <f t="shared" si="1"/>
         <v>21.1</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F44">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G44">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F47">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G47">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A45" s="2" t="s">
+    <row r="48" spans="1:7" ht="21" x14ac:dyDescent="0.35">
+      <c r="A48" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="F45">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G45">
+      <c r="F48">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G48">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B46" s="1" t="s">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B49" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="C49" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D46" s="1" t="s">
+      <c r="D49" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E46" s="1" t="s">
+      <c r="E49" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F46" s="1" t="s">
+      <c r="F49" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G46" s="1" t="s">
+      <c r="G49" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>86</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B50" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C50" t="s">
         <v>88</v>
       </c>
-      <c r="D47">
+      <c r="D50">
         <v>40</v>
       </c>
-      <c r="E47">
+      <c r="E50">
         <v>10</v>
       </c>
-      <c r="F47">
+      <c r="F50">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="G47" t="e">
-        <f>(C47*F47)</f>
+      <c r="G50" t="e">
+        <f>(C50*F50)</f>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>89</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B51" t="s">
         <v>90</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C51" t="s">
         <v>88</v>
       </c>
-      <c r="D48">
+      <c r="D51">
         <v>20</v>
       </c>
-      <c r="E48">
+      <c r="E51">
         <v>5</v>
       </c>
-      <c r="F48">
+      <c r="F51">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="G48" t="e">
+      <c r="G51" t="e">
         <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A50" s="2" t="s">
+    <row r="53" spans="1:7" ht="21" x14ac:dyDescent="0.35">
+      <c r="A53" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B51" s="1" t="s">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B54" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="C54" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D51" s="1" t="s">
+      <c r="D54" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E51" s="1" t="s">
+      <c r="E54" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F51" s="1" t="s">
+      <c r="F54" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G51" s="1" t="s">
+      <c r="G54" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>92</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B55" t="s">
         <v>93</v>
       </c>
-      <c r="C52">
+      <c r="C55">
         <v>1.96</v>
       </c>
-      <c r="D52">
+      <c r="D55">
         <v>12</v>
       </c>
-      <c r="E52">
+      <c r="E55">
         <v>6</v>
       </c>
-      <c r="F52">
+      <c r="F55">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="G52">
+      <c r="G55">
         <f t="shared" si="1"/>
         <v>35.28</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>94</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B56" t="s">
         <v>95</v>
       </c>
-      <c r="C53">
+      <c r="C56">
         <v>6.27</v>
       </c>
-      <c r="D53">
+      <c r="D56">
         <v>8</v>
       </c>
-      <c r="E53">
+      <c r="E56">
         <v>2</v>
       </c>
-      <c r="F53">
+      <c r="F56">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G53">
+      <c r="G56">
         <f t="shared" si="1"/>
         <v>62.699999999999996</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>97</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B57" t="s">
         <v>96</v>
       </c>
-      <c r="C54">
+      <c r="C57">
         <v>3.05</v>
       </c>
-      <c r="D54">
+      <c r="D57">
         <v>6</v>
       </c>
-      <c r="E54">
+      <c r="E57">
         <v>2</v>
       </c>
-      <c r="F54">
+      <c r="F57">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="G54">
+      <c r="G57">
         <f t="shared" si="1"/>
         <v>24.4</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>98</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B58" t="s">
         <v>99</v>
       </c>
-      <c r="C55">
+      <c r="C58">
         <v>4.6399999999999997</v>
       </c>
-      <c r="D55">
+      <c r="D58">
         <v>12</v>
       </c>
-      <c r="E55">
+      <c r="E58">
         <v>4</v>
       </c>
-      <c r="F55">
+      <c r="F58">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="G55">
+      <c r="G58">
         <f t="shared" si="1"/>
         <v>74.239999999999995</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
         <v>100</v>
       </c>
-      <c r="B56" s="5" t="s">
+      <c r="B59" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C56">
+      <c r="C59">
         <v>4.6399999999999997</v>
       </c>
-      <c r="D56">
-        <v>0</v>
-      </c>
-      <c r="E56">
+      <c r="D59">
+        <v>0</v>
+      </c>
+      <c r="E59">
         <v>2</v>
       </c>
-      <c r="F56">
+      <c r="F59">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G56">
+      <c r="G59">
         <f t="shared" si="1"/>
         <v>9.2799999999999994</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
         <v>102</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B60" t="s">
         <v>103</v>
       </c>
-      <c r="C57">
+      <c r="C60">
         <v>12.29</v>
       </c>
-      <c r="D57">
+      <c r="D60">
         <v>10</v>
       </c>
-      <c r="E57">
+      <c r="E60">
         <v>4</v>
       </c>
-      <c r="F57">
+      <c r="F60">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="G57">
+      <c r="G60">
         <f t="shared" si="1"/>
         <v>172.06</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
         <v>120</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B61" t="s">
         <v>121</v>
       </c>
-      <c r="C58">
+      <c r="C61">
         <v>16.48</v>
       </c>
-      <c r="D58">
-        <v>1</v>
-      </c>
-      <c r="E58">
-        <v>0</v>
-      </c>
-      <c r="F58">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="G58">
+      <c r="D61">
+        <v>1</v>
+      </c>
+      <c r="E61">
+        <v>0</v>
+      </c>
+      <c r="F61">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G61">
         <f t="shared" si="1"/>
         <v>16.48</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
         <v>122</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B62" t="s">
         <v>123</v>
       </c>
-      <c r="C59">
+      <c r="C62">
         <v>2.06</v>
       </c>
-      <c r="D59">
-        <v>1</v>
-      </c>
-      <c r="E59">
-        <v>0</v>
-      </c>
-      <c r="F59">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="G59">
+      <c r="D62">
+        <v>1</v>
+      </c>
+      <c r="E62">
+        <v>0</v>
+      </c>
+      <c r="F62">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G62">
         <f t="shared" si="1"/>
         <v>2.06</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>105</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B63" t="s">
         <v>104</v>
       </c>
-      <c r="C60">
+      <c r="C63">
         <v>6.7</v>
       </c>
-      <c r="D60">
-        <v>0</v>
-      </c>
-      <c r="E60">
+      <c r="D63">
+        <v>0</v>
+      </c>
+      <c r="E63">
         <v>2</v>
       </c>
-      <c r="F60">
+      <c r="F63">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G60">
+      <c r="G63">
         <f t="shared" si="1"/>
         <v>13.4</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
         <v>106</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B64" t="s">
         <v>107</v>
       </c>
-      <c r="C61">
+      <c r="C64">
         <v>18.16</v>
       </c>
-      <c r="D61">
+      <c r="D64">
         <v>4</v>
       </c>
-      <c r="E61">
+      <c r="E64">
         <v>4</v>
       </c>
-      <c r="F61">
+      <c r="F64">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="G61">
+      <c r="G64">
         <f t="shared" si="1"/>
         <v>145.28</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
         <v>108</v>
       </c>
-      <c r="B62">
+      <c r="B65">
         <v>17555</v>
       </c>
-      <c r="C62">
+      <c r="C65">
         <v>106.81</v>
       </c>
-      <c r="D62">
-        <v>0</v>
-      </c>
-      <c r="E62">
-        <v>1</v>
-      </c>
-      <c r="F62">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="G62">
+      <c r="D65">
+        <v>0</v>
+      </c>
+      <c r="E65">
+        <v>1</v>
+      </c>
+      <c r="F65">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G65">
         <f t="shared" si="1"/>
         <v>106.81</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A66" s="2" t="s">
+    <row r="69" spans="1:7" ht="21" x14ac:dyDescent="0.35">
+      <c r="A69" s="2" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B67" s="1" t="s">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B70" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C67" s="1" t="s">
+      <c r="C70" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D67" s="1" t="s">
+      <c r="D70" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E67" s="1" t="s">
+      <c r="E70" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F67" s="1" t="s">
+      <c r="F70" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G67" s="1" t="s">
+      <c r="G70" s="1" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>112</v>
-      </c>
-      <c r="B68" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="C68">
-        <v>9</v>
-      </c>
-      <c r="D68">
-        <v>4</v>
-      </c>
-      <c r="E68">
-        <v>1</v>
-      </c>
-      <c r="F68">
-        <f t="shared" ref="F68:F86" si="4">(D68+E68)</f>
-        <v>5</v>
-      </c>
-      <c r="G68">
-        <f t="shared" ref="G68:G86" si="5">(C68*F68)</f>
-        <v>45</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>114</v>
-      </c>
-      <c r="B69" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="C69">
-        <v>9.4</v>
-      </c>
-      <c r="D69">
-        <v>3</v>
-      </c>
-      <c r="E69">
-        <v>0</v>
-      </c>
-      <c r="F69">
-        <f t="shared" si="4"/>
-        <v>3</v>
-      </c>
-      <c r="G69">
-        <f t="shared" si="5"/>
-        <v>28.200000000000003</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>117</v>
-      </c>
-      <c r="B70" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="C70">
-        <v>3.6</v>
-      </c>
-      <c r="D70">
-        <v>3</v>
-      </c>
-      <c r="E70">
-        <v>3</v>
-      </c>
-      <c r="F70">
-        <f t="shared" si="4"/>
-        <v>6</v>
-      </c>
-      <c r="G70">
-        <f t="shared" si="5"/>
-        <v>21.6</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="C71">
         <v>9</v>
       </c>
       <c r="D71">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E71">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F71">
-        <f t="shared" si="4"/>
-        <v>4</v>
+        <f t="shared" ref="F71:F91" si="4">(D71+E71)</f>
+        <v>5</v>
       </c>
       <c r="G71">
-        <f t="shared" si="5"/>
-        <v>36</v>
+        <f t="shared" ref="G71:G91" si="5">(C71*F71)</f>
+        <v>45</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="C72">
-        <v>2.9</v>
+        <v>9.4</v>
       </c>
       <c r="D72">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E72">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F72">
         <f t="shared" si="4"/>
@@ -2503,721 +2565,721 @@
       </c>
       <c r="G72">
         <f t="shared" si="5"/>
-        <v>8.6999999999999993</v>
+        <v>28.200000000000003</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>126</v>
+        <v>236</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>127</v>
+        <v>237</v>
       </c>
       <c r="C73">
-        <v>1.7</v>
+        <v>6.9</v>
       </c>
       <c r="D73">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E73">
+        <v>0</v>
+      </c>
+      <c r="F73">
+        <f t="shared" ref="F73" si="6">(D73+E73)</f>
+        <v>6</v>
+      </c>
+      <c r="G73">
+        <f t="shared" ref="G73" si="7">(C73*F73)</f>
+        <v>41.400000000000006</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>239</v>
+      </c>
+      <c r="B74" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="C74">
+        <v>7.5</v>
+      </c>
+      <c r="D74">
+        <v>6</v>
+      </c>
+      <c r="E74">
+        <v>0</v>
+      </c>
+      <c r="F74">
+        <f t="shared" ref="F74" si="8">(D74+E74)</f>
+        <v>6</v>
+      </c>
+      <c r="G74">
+        <f t="shared" ref="G74" si="9">(C74*F74)</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>117</v>
+      </c>
+      <c r="B75" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="C75">
+        <v>3.6</v>
+      </c>
+      <c r="D75">
         <v>3</v>
       </c>
-      <c r="F73">
+      <c r="E75">
+        <v>3</v>
+      </c>
+      <c r="F75">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="G75">
+        <f t="shared" si="5"/>
+        <v>21.6</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>118</v>
+      </c>
+      <c r="B76" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="C76">
+        <v>9</v>
+      </c>
+      <c r="D76">
+        <v>2</v>
+      </c>
+      <c r="E76">
+        <v>2</v>
+      </c>
+      <c r="F76">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="G73">
+      <c r="G76">
+        <f t="shared" si="5"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>124</v>
+      </c>
+      <c r="B77" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="C77">
+        <v>2.9</v>
+      </c>
+      <c r="D77">
+        <v>1</v>
+      </c>
+      <c r="E77">
+        <v>2</v>
+      </c>
+      <c r="F77">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="G77">
+        <f t="shared" si="5"/>
+        <v>8.6999999999999993</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>126</v>
+      </c>
+      <c r="B78" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="C78">
+        <v>1.7</v>
+      </c>
+      <c r="D78">
+        <v>1</v>
+      </c>
+      <c r="E78">
+        <v>3</v>
+      </c>
+      <c r="F78">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="G78">
         <f t="shared" si="5"/>
         <v>6.8</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
         <v>128</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B79" t="s">
         <v>129</v>
       </c>
-      <c r="C74">
+      <c r="C79">
         <v>1.7</v>
       </c>
-      <c r="D74">
-        <v>0</v>
-      </c>
-      <c r="E74">
+      <c r="D79">
+        <v>0</v>
+      </c>
+      <c r="E79">
         <v>2</v>
       </c>
-      <c r="F74">
+      <c r="F79">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="G74">
+      <c r="G79">
         <f t="shared" si="5"/>
         <v>3.4</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
         <v>130</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B80" t="s">
         <v>131</v>
       </c>
-      <c r="C75">
+      <c r="C80">
         <v>2.8</v>
       </c>
-      <c r="D75">
-        <v>1</v>
-      </c>
-      <c r="E75">
+      <c r="D80">
+        <v>1</v>
+      </c>
+      <c r="E80">
         <v>2</v>
       </c>
-      <c r="F75">
+      <c r="F80">
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
-      <c r="G75">
+      <c r="G80">
         <f t="shared" si="5"/>
         <v>8.3999999999999986</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
         <v>132</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B81" t="s">
         <v>133</v>
       </c>
-      <c r="C76">
+      <c r="C81">
         <v>2.2000000000000002</v>
       </c>
-      <c r="D76">
+      <c r="D81">
         <v>4</v>
       </c>
-      <c r="E76">
+      <c r="E81">
         <v>4</v>
       </c>
-      <c r="F76">
+      <c r="F81">
         <f t="shared" si="4"/>
         <v>8</v>
       </c>
-      <c r="G76">
+      <c r="G81">
         <f t="shared" si="5"/>
         <v>17.600000000000001</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
         <v>135</v>
       </c>
-      <c r="B77" s="6" t="s">
+      <c r="B82" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="C77">
+      <c r="C82">
         <v>96.4</v>
       </c>
-      <c r="D77">
-        <v>1</v>
-      </c>
-      <c r="E77">
-        <v>0</v>
-      </c>
-      <c r="F77">
+      <c r="D82">
+        <v>1</v>
+      </c>
+      <c r="E82">
+        <v>0</v>
+      </c>
+      <c r="F82">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="G77">
+      <c r="G82">
         <f t="shared" si="5"/>
         <v>96.4</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
         <v>136</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B83" t="s">
         <v>137</v>
       </c>
-      <c r="C78">
+      <c r="C83">
         <v>129.9</v>
       </c>
-      <c r="D78">
-        <v>1</v>
-      </c>
-      <c r="E78">
-        <v>0</v>
-      </c>
-      <c r="F78">
+      <c r="D83">
+        <v>1</v>
+      </c>
+      <c r="E83">
+        <v>0</v>
+      </c>
+      <c r="F83">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="G78">
+      <c r="G83">
         <f t="shared" si="5"/>
         <v>129.9</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
         <v>138</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B84" t="s">
         <v>139</v>
       </c>
-      <c r="C79">
+      <c r="C84">
         <v>46.4</v>
       </c>
-      <c r="D79">
-        <v>1</v>
-      </c>
-      <c r="E79">
-        <v>0</v>
-      </c>
-      <c r="F79">
+      <c r="D84">
+        <v>1</v>
+      </c>
+      <c r="E84">
+        <v>0</v>
+      </c>
+      <c r="F84">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="G79">
+      <c r="G84">
         <f t="shared" si="5"/>
         <v>46.4</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
         <v>140</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B85" t="s">
         <v>141</v>
       </c>
-      <c r="C80">
+      <c r="C85">
         <v>34.9</v>
       </c>
-      <c r="D80">
-        <v>1</v>
-      </c>
-      <c r="E80">
-        <v>0</v>
-      </c>
-      <c r="F80">
+      <c r="D85">
+        <v>1</v>
+      </c>
+      <c r="E85">
+        <v>0</v>
+      </c>
+      <c r="F85">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="G80">
+      <c r="G85">
         <f t="shared" si="5"/>
         <v>34.9</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
         <v>144</v>
       </c>
-      <c r="B81" s="6" t="s">
+      <c r="B86" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="C81">
+      <c r="C86">
         <v>44.1</v>
       </c>
-      <c r="D81">
-        <v>1</v>
-      </c>
-      <c r="E81">
-        <v>0</v>
-      </c>
-      <c r="F81">
+      <c r="D86">
+        <v>1</v>
+      </c>
+      <c r="E86">
+        <v>0</v>
+      </c>
+      <c r="F86">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="G81">
+      <c r="G86">
         <f t="shared" si="5"/>
         <v>44.1</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
         <v>143</v>
       </c>
-      <c r="B82" s="6" t="s">
+      <c r="B87" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="C82">
+      <c r="C87">
         <v>3.4</v>
       </c>
-      <c r="D82">
-        <v>1</v>
-      </c>
-      <c r="E82">
-        <v>1</v>
-      </c>
-      <c r="F82">
+      <c r="D87">
+        <v>1</v>
+      </c>
+      <c r="E87">
+        <v>1</v>
+      </c>
+      <c r="F87">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="G82">
+      <c r="G87">
         <f t="shared" si="5"/>
         <v>6.8</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
         <v>146</v>
       </c>
-      <c r="B83" s="6" t="s">
+      <c r="B88" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="C83">
+      <c r="C88">
         <v>3.4</v>
       </c>
-      <c r="D83">
-        <v>1</v>
-      </c>
-      <c r="E83">
-        <v>1</v>
-      </c>
-      <c r="F83">
+      <c r="D88">
+        <v>1</v>
+      </c>
+      <c r="E88">
+        <v>1</v>
+      </c>
+      <c r="F88">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="G83">
+      <c r="G88">
         <f t="shared" si="5"/>
         <v>6.8</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
         <v>149</v>
       </c>
-      <c r="B84" s="6" t="s">
+      <c r="B89" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="C84">
+      <c r="C89">
         <v>5.2</v>
       </c>
-      <c r="D84">
-        <v>0</v>
-      </c>
-      <c r="E84">
-        <v>1</v>
-      </c>
-      <c r="F84">
+      <c r="D89">
+        <v>0</v>
+      </c>
+      <c r="E89">
+        <v>1</v>
+      </c>
+      <c r="F89">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="G84">
+      <c r="G89">
         <f t="shared" si="5"/>
         <v>5.2</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
         <v>150</v>
       </c>
-      <c r="B85" s="6" t="s">
+      <c r="B90" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="C85">
+      <c r="C90">
         <v>0.74</v>
       </c>
-      <c r="D85">
-        <v>0</v>
-      </c>
-      <c r="E85">
+      <c r="D90">
+        <v>0</v>
+      </c>
+      <c r="E90">
         <v>10</v>
       </c>
-      <c r="F85">
+      <c r="F90">
         <f t="shared" si="4"/>
         <v>10</v>
       </c>
-      <c r="G85">
+      <c r="G90">
         <f t="shared" si="5"/>
         <v>7.4</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
         <v>153</v>
       </c>
-      <c r="B86" s="6" t="s">
+      <c r="B91" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="C86">
+      <c r="C91">
         <v>0.76</v>
       </c>
-      <c r="D86">
-        <v>0</v>
-      </c>
-      <c r="E86">
+      <c r="D91">
+        <v>0</v>
+      </c>
+      <c r="E91">
         <v>10</v>
       </c>
-      <c r="F86">
+      <c r="F91">
         <f t="shared" si="4"/>
         <v>10</v>
       </c>
-      <c r="G86">
+      <c r="G91">
         <f t="shared" si="5"/>
         <v>7.6</v>
       </c>
     </row>
-    <row r="88" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A88" s="2" t="s">
+    <row r="93" spans="1:7" ht="21" x14ac:dyDescent="0.35">
+      <c r="A93" s="2" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A89" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B89" s="1" t="s">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B94" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C89" s="1" t="s">
+      <c r="C94" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D89" s="1" t="s">
+      <c r="D94" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E89" s="1" t="s">
+      <c r="E94" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F89" s="1" t="s">
+      <c r="F94" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G89" s="1" t="s">
+      <c r="G94" s="1" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>154</v>
-      </c>
-      <c r="B90" t="s">
-        <v>175</v>
-      </c>
-      <c r="C90">
-        <v>8.32</v>
-      </c>
-      <c r="D90">
-        <v>3</v>
-      </c>
-      <c r="E90">
-        <v>1</v>
-      </c>
-      <c r="F90">
-        <f t="shared" ref="F90" si="6">(D90+E90)</f>
-        <v>4</v>
-      </c>
-      <c r="G90">
-        <f t="shared" ref="G90" si="7">(C90*F90)</f>
-        <v>33.28</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>155</v>
-      </c>
-      <c r="B91" t="s">
-        <v>156</v>
-      </c>
-      <c r="C91">
-        <v>43.38</v>
-      </c>
-      <c r="D91">
-        <v>1</v>
-      </c>
-      <c r="E91">
-        <v>0</v>
-      </c>
-      <c r="F91">
-        <f t="shared" ref="F91:F99" si="8">(D91+E91)</f>
-        <v>1</v>
-      </c>
-      <c r="G91">
-        <f t="shared" ref="G91:G99" si="9">(C91*F91)</f>
-        <v>43.38</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>157</v>
-      </c>
-      <c r="B92" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="C92">
-        <v>1.21</v>
-      </c>
-      <c r="D92">
-        <v>50</v>
-      </c>
-      <c r="E92">
-        <v>0</v>
-      </c>
-      <c r="F92">
-        <f t="shared" si="8"/>
-        <v>50</v>
-      </c>
-      <c r="G92">
-        <f t="shared" si="9"/>
-        <v>60.5</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>159</v>
-      </c>
-      <c r="B93" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="C93">
-        <v>0.43</v>
-      </c>
-      <c r="D93">
-        <v>25</v>
-      </c>
-      <c r="E93">
-        <v>0</v>
-      </c>
-      <c r="F93">
-        <f t="shared" si="8"/>
-        <v>25</v>
-      </c>
-      <c r="G93">
-        <f t="shared" si="9"/>
-        <v>10.75</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>161</v>
-      </c>
-      <c r="B94" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="C94">
-        <v>9.08</v>
-      </c>
-      <c r="D94">
-        <v>1</v>
-      </c>
-      <c r="E94">
-        <v>0</v>
-      </c>
-      <c r="F94">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="G94">
-        <f t="shared" si="9"/>
-        <v>9.08</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>163</v>
-      </c>
-      <c r="B95" s="6" t="s">
-        <v>164</v>
+        <v>154</v>
+      </c>
+      <c r="B95" t="s">
+        <v>175</v>
       </c>
       <c r="C95">
-        <v>4.01</v>
+        <v>8.32</v>
       </c>
       <c r="D95">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E95">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F95">
-        <f t="shared" si="8"/>
-        <v>1</v>
+        <f t="shared" ref="F95" si="10">(D95+E95)</f>
+        <v>4</v>
       </c>
       <c r="G95">
-        <f t="shared" si="9"/>
-        <v>4.01</v>
+        <f t="shared" ref="G95" si="11">(C95*F95)</f>
+        <v>33.28</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="B96" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="C96">
-        <v>12.32</v>
+        <v>43.38</v>
       </c>
       <c r="D96">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E96">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F96">
-        <f t="shared" si="8"/>
+        <f t="shared" ref="F96:F105" si="12">(D96+E96)</f>
         <v>1</v>
       </c>
       <c r="G96">
-        <f t="shared" si="9"/>
-        <v>12.32</v>
+        <f t="shared" ref="G96:G105" si="13">(C96*F96)</f>
+        <v>43.38</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="B97" s="6" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="C97">
-        <v>6.65</v>
+        <v>1.21</v>
       </c>
       <c r="D97">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="E97">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F97">
-        <f t="shared" si="8"/>
-        <v>2</v>
+        <f t="shared" si="12"/>
+        <v>50</v>
       </c>
       <c r="G97">
-        <f t="shared" si="9"/>
-        <v>13.3</v>
+        <f t="shared" si="13"/>
+        <v>60.5</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="B98" s="6" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="C98">
-        <v>5.6</v>
+        <v>0.43</v>
       </c>
       <c r="D98">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="E98">
         <v>0</v>
       </c>
       <c r="F98">
-        <f t="shared" si="8"/>
-        <v>1</v>
+        <f t="shared" si="12"/>
+        <v>25</v>
       </c>
       <c r="G98">
-        <f t="shared" si="9"/>
-        <v>5.6</v>
+        <f t="shared" si="13"/>
+        <v>10.75</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="B99" s="6" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="C99">
-        <v>5.45</v>
+        <v>9.08</v>
       </c>
       <c r="D99">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E99">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F99">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="G99">
-        <f t="shared" si="9"/>
-        <v>5.45</v>
+        <f t="shared" si="13"/>
+        <v>9.08</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="B100" s="6" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="C100">
-        <v>0.39</v>
+        <v>4.01</v>
       </c>
       <c r="D100">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="E100">
         <v>0</v>
       </c>
       <c r="F100">
-        <f t="shared" ref="F100:F107" si="10">(D100+E100)</f>
-        <v>50</v>
+        <f t="shared" si="12"/>
+        <v>1</v>
       </c>
       <c r="G100">
-        <f t="shared" ref="G100:G107" si="11">(C100*F100)</f>
-        <v>19.5</v>
+        <f t="shared" si="13"/>
+        <v>4.01</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>188</v>
-      </c>
-      <c r="B101" s="6" t="s">
-        <v>190</v>
+        <v>165</v>
+      </c>
+      <c r="B101" t="s">
+        <v>166</v>
       </c>
       <c r="C101">
-        <v>4.99</v>
+        <v>12.32</v>
       </c>
       <c r="D101">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E101">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F101">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="G101">
-        <f t="shared" si="11"/>
-        <v>4.99</v>
+        <f t="shared" si="13"/>
+        <v>12.32</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>189</v>
+        <v>167</v>
       </c>
       <c r="B102" s="6" t="s">
-        <v>191</v>
+        <v>168</v>
       </c>
       <c r="C102">
-        <v>5.01</v>
+        <v>6.65</v>
       </c>
       <c r="D102">
         <v>1</v>
       </c>
       <c r="E102">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F102">
-        <f t="shared" si="10"/>
-        <v>1</v>
+        <f t="shared" si="12"/>
+        <v>2</v>
       </c>
       <c r="G102">
-        <f t="shared" si="11"/>
-        <v>5.01</v>
+        <f t="shared" si="13"/>
+        <v>13.3</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>193</v>
+        <v>169</v>
       </c>
       <c r="B103" s="6" t="s">
-        <v>194</v>
+        <v>170</v>
       </c>
       <c r="C103">
-        <v>5.65</v>
+        <v>5.6</v>
       </c>
       <c r="D103">
         <v>1</v>
@@ -3226,48 +3288,48 @@
         <v>0</v>
       </c>
       <c r="F103">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="G103">
-        <f t="shared" si="11"/>
-        <v>5.65</v>
+        <f t="shared" si="13"/>
+        <v>5.6</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>195</v>
+        <v>171</v>
       </c>
       <c r="B104" s="6" t="s">
-        <v>196</v>
+        <v>172</v>
       </c>
       <c r="C104">
-        <v>7.08</v>
+        <v>5.45</v>
       </c>
       <c r="D104">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E104">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F104">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="G104">
-        <f t="shared" si="11"/>
-        <v>7.08</v>
+        <f t="shared" si="13"/>
+        <v>5.45</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>197</v>
+        <v>242</v>
       </c>
       <c r="B105" s="6" t="s">
-        <v>198</v>
+        <v>243</v>
       </c>
       <c r="C105">
-        <v>2.87</v>
+        <v>5.89</v>
       </c>
       <c r="D105">
         <v>1</v>
@@ -3276,23 +3338,23 @@
         <v>0</v>
       </c>
       <c r="F105">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="G105">
-        <f t="shared" si="11"/>
-        <v>2.87</v>
+        <f t="shared" si="13"/>
+        <v>5.89</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>199</v>
+        <v>244</v>
       </c>
       <c r="B106" s="6" t="s">
-        <v>200</v>
+        <v>245</v>
       </c>
       <c r="C106">
-        <v>3.13</v>
+        <v>5.28</v>
       </c>
       <c r="D106">
         <v>1</v>
@@ -3301,76 +3363,123 @@
         <v>0</v>
       </c>
       <c r="F106">
-        <f t="shared" si="10"/>
+        <f t="shared" ref="F106" si="14">(D106+E106)</f>
         <v>1</v>
       </c>
       <c r="G106">
-        <f t="shared" si="11"/>
-        <v>3.13</v>
+        <f t="shared" ref="G106" si="15">(C106*F106)</f>
+        <v>5.28</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>201</v>
-      </c>
-      <c r="B107" t="s">
-        <v>202</v>
+        <v>173</v>
+      </c>
+      <c r="B107" s="6" t="s">
+        <v>174</v>
       </c>
       <c r="C107">
-        <v>13.94</v>
+        <v>0.39</v>
       </c>
       <c r="D107">
-        <v>2</v>
+        <v>50</v>
       </c>
       <c r="E107">
         <v>0</v>
       </c>
       <c r="F107">
-        <f t="shared" si="10"/>
-        <v>2</v>
+        <f t="shared" ref="F107:F114" si="16">(D107+E107)</f>
+        <v>50</v>
       </c>
       <c r="G107">
-        <f t="shared" si="11"/>
-        <v>27.88</v>
-      </c>
-    </row>
-    <row r="109" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A109" s="2" t="s">
-        <v>204</v>
+        <f t="shared" ref="G107:G114" si="17">(C107*F107)</f>
+        <v>19.5</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>188</v>
+      </c>
+      <c r="B108" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="C108">
+        <v>4.99</v>
+      </c>
+      <c r="D108">
+        <v>1</v>
+      </c>
+      <c r="E108">
+        <v>0</v>
+      </c>
+      <c r="F108">
+        <f t="shared" si="16"/>
+        <v>1</v>
+      </c>
+      <c r="G108">
+        <f t="shared" si="17"/>
+        <v>4.99</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>189</v>
+      </c>
+      <c r="B109" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="C109">
+        <v>5.01</v>
+      </c>
+      <c r="D109">
+        <v>1</v>
+      </c>
+      <c r="E109">
+        <v>0</v>
+      </c>
+      <c r="F109">
+        <f t="shared" si="16"/>
+        <v>1</v>
+      </c>
+      <c r="G109">
+        <f t="shared" si="17"/>
+        <v>5.01</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A110" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B110" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C110" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D110" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E110" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F110" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G110" s="1" t="s">
-        <v>40</v>
+      <c r="A110" t="s">
+        <v>193</v>
+      </c>
+      <c r="B110" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="C110">
+        <v>5.65</v>
+      </c>
+      <c r="D110">
+        <v>1</v>
+      </c>
+      <c r="E110">
+        <v>0</v>
+      </c>
+      <c r="F110">
+        <f t="shared" si="16"/>
+        <v>1</v>
+      </c>
+      <c r="G110">
+        <f t="shared" si="17"/>
+        <v>5.65</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>206</v>
-      </c>
-      <c r="B111" s="7" t="s">
-        <v>205</v>
+        <v>195</v>
+      </c>
+      <c r="B111" s="6" t="s">
+        <v>196</v>
       </c>
       <c r="C111">
-        <v>381.45</v>
+        <v>7.08</v>
       </c>
       <c r="D111">
         <v>1</v>
@@ -3379,214 +3488,266 @@
         <v>0</v>
       </c>
       <c r="F111">
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="G111">
-        <v>381.45</v>
+        <f t="shared" si="17"/>
+        <v>7.08</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
+        <v>197</v>
+      </c>
+      <c r="B112" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="C112">
+        <v>2.87</v>
+      </c>
+      <c r="D112">
+        <v>1</v>
+      </c>
+      <c r="E112">
+        <v>0</v>
+      </c>
+      <c r="F112">
+        <f t="shared" si="16"/>
+        <v>1</v>
+      </c>
+      <c r="G112">
+        <f t="shared" si="17"/>
+        <v>2.87</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>199</v>
+      </c>
+      <c r="B113" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="C113">
+        <v>3.13</v>
+      </c>
+      <c r="D113">
+        <v>1</v>
+      </c>
+      <c r="E113">
+        <v>0</v>
+      </c>
+      <c r="F113">
+        <f t="shared" si="16"/>
+        <v>1</v>
+      </c>
+      <c r="G113">
+        <f t="shared" si="17"/>
+        <v>3.13</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>201</v>
+      </c>
+      <c r="B114" t="s">
+        <v>202</v>
+      </c>
+      <c r="C114">
+        <v>13.94</v>
+      </c>
+      <c r="D114">
+        <v>2</v>
+      </c>
+      <c r="E114">
+        <v>0</v>
+      </c>
+      <c r="F114">
+        <f t="shared" si="16"/>
+        <v>2</v>
+      </c>
+      <c r="G114">
+        <f t="shared" si="17"/>
+        <v>27.88</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A117" s="2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A118" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D118" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E118" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F118" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G118" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>206</v>
+      </c>
+      <c r="B119" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="C119">
+        <v>381.45</v>
+      </c>
+      <c r="D119">
+        <v>1</v>
+      </c>
+      <c r="E119">
+        <v>0</v>
+      </c>
+      <c r="F119">
+        <v>1</v>
+      </c>
+      <c r="G119">
+        <v>381.45</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
         <v>221</v>
       </c>
-      <c r="B112" s="7" t="s">
+      <c r="B120" s="7" t="s">
         <v>205</v>
       </c>
-      <c r="C112">
+      <c r="C120">
         <v>1702.97</v>
       </c>
-      <c r="D112">
-        <v>1</v>
-      </c>
-      <c r="E112">
-        <v>0</v>
-      </c>
-      <c r="F112">
-        <v>1</v>
-      </c>
-      <c r="G112">
+      <c r="D120">
+        <v>1</v>
+      </c>
+      <c r="E120">
+        <v>0</v>
+      </c>
+      <c r="F120">
+        <v>1</v>
+      </c>
+      <c r="G120">
         <v>1702.97</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B113" s="6"/>
-    </row>
-    <row r="114" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A114" s="2" t="s">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B121" s="6"/>
+    </row>
+    <row r="122" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A122" s="2" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A115" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B115" s="1" t="s">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A123" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B123" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C115" s="1" t="s">
+      <c r="C123" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D115" s="1" t="s">
+      <c r="D123" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E115" s="1" t="s">
+      <c r="E123" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F115" s="1" t="s">
+      <c r="F123" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G115" s="1" t="s">
+      <c r="G123" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A116" s="5" t="s">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A124" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="B116" t="s">
+      <c r="B124" t="s">
         <v>184</v>
       </c>
-      <c r="C116" s="5">
+      <c r="C124" s="5">
         <v>169</v>
       </c>
-      <c r="D116" s="5">
+      <c r="D124" s="5">
         <v>2</v>
       </c>
-      <c r="E116" s="5">
-        <v>0</v>
-      </c>
-      <c r="F116">
-        <f t="shared" ref="F116" si="12">(D116+E116)</f>
+      <c r="E124" s="5">
+        <v>0</v>
+      </c>
+      <c r="F124">
+        <f t="shared" ref="F124" si="18">(D124+E124)</f>
         <v>2</v>
       </c>
-      <c r="G116">
-        <f t="shared" ref="G116" si="13">(C116*F116)</f>
+      <c r="G124">
+        <f t="shared" ref="G124" si="19">(C124*F124)</f>
         <v>338</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A117" s="1"/>
-      <c r="B117" s="1"/>
-      <c r="C117" s="1"/>
-      <c r="D117" s="1"/>
-      <c r="E117" s="1"/>
-      <c r="F117" s="1"/>
-      <c r="G117" s="1"/>
-    </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A118" s="1"/>
-      <c r="B118" s="1"/>
-      <c r="C118" s="1"/>
-      <c r="D118" s="1"/>
-      <c r="E118" s="1"/>
-      <c r="F118" s="1"/>
-      <c r="G118" s="1"/>
-    </row>
-    <row r="119" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A119" s="2" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
-        <v>180</v>
-      </c>
-      <c r="B121" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
-        <v>181</v>
-      </c>
-      <c r="B122" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="124" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A124" s="2" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A125" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B125" s="1" t="s">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A125" s="1"/>
+      <c r="B125" s="1"/>
+      <c r="C125" s="1"/>
+      <c r="D125" s="1"/>
+      <c r="E125" s="1"/>
+      <c r="F125" s="1"/>
+      <c r="G125" s="1"/>
+    </row>
+    <row r="126" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A126" s="2" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A127" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B127" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C125" s="1" t="s">
+      <c r="C127" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D125" s="1" t="s">
+      <c r="D127" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E125" s="1" t="s">
+      <c r="E127" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F125" s="1" t="s">
+      <c r="F127" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G125" s="1" t="s">
+      <c r="G127" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A126" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="B126" t="s">
-        <v>208</v>
-      </c>
-      <c r="C126" s="5">
-        <v>852</v>
-      </c>
-      <c r="D126" s="5">
-        <v>3</v>
-      </c>
-      <c r="E126" s="5">
-        <v>0</v>
-      </c>
-      <c r="F126">
-        <f>(D126+E126)</f>
-        <v>3</v>
-      </c>
-      <c r="G126">
-        <f t="shared" ref="G126" si="14">(C126*F126)</f>
-        <v>2556</v>
-      </c>
-    </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A127" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="B127" t="s">
-        <v>211</v>
-      </c>
-      <c r="C127" s="5"/>
-      <c r="D127" s="5">
-        <v>1</v>
-      </c>
-      <c r="E127" s="5">
-        <v>0</v>
-      </c>
-      <c r="F127">
-        <f t="shared" ref="F127:F129" si="15">(D127+E127)</f>
-        <v>1</v>
-      </c>
-      <c r="G127">
-        <f t="shared" ref="G127:G129" si="16">(C127*F127)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" s="5" t="s">
-        <v>212</v>
+        <v>233</v>
       </c>
       <c r="B128" t="s">
-        <v>213</v>
-      </c>
-      <c r="C128" s="5"/>
+        <v>232</v>
+      </c>
+      <c r="C128" s="5">
+        <v>540</v>
+      </c>
       <c r="D128" s="5">
         <v>2</v>
       </c>
@@ -3594,150 +3755,312 @@
         <v>0</v>
       </c>
       <c r="F128">
-        <f t="shared" si="15"/>
+        <f>(D128+E128)</f>
         <v>2</v>
       </c>
       <c r="G128">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+        <f>(C128*F128)</f>
+        <v>1080</v>
+      </c>
+      <c r="H128" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="B129" t="s">
+        <v>235</v>
+      </c>
+      <c r="C129" s="5">
+        <v>675</v>
+      </c>
+      <c r="D129" s="5">
+        <v>1</v>
+      </c>
+      <c r="E129" s="5">
+        <v>0</v>
+      </c>
+      <c r="F129">
+        <f>(D129+E129)</f>
+        <v>1</v>
+      </c>
+      <c r="G129">
+        <f>(C129*F129)</f>
+        <v>675</v>
+      </c>
+      <c r="H129" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A130" s="1"/>
+      <c r="B130" s="1"/>
+      <c r="C130" s="1"/>
+      <c r="D130" s="1"/>
+      <c r="E130" s="1"/>
+      <c r="F130" s="1"/>
+      <c r="G130" s="1"/>
+    </row>
+    <row r="131" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A131" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>180</v>
+      </c>
+      <c r="B133" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>181</v>
+      </c>
+      <c r="B134" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A136" s="2" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A137" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D137" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E137" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F137" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G137" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A138" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="B138" t="s">
+        <v>208</v>
+      </c>
+      <c r="C138" s="5">
+        <v>852</v>
+      </c>
+      <c r="D138" s="5">
+        <v>3</v>
+      </c>
+      <c r="E138" s="5">
+        <v>0</v>
+      </c>
+      <c r="F138">
+        <f>(D138+E138)</f>
+        <v>3</v>
+      </c>
+      <c r="G138">
+        <f t="shared" ref="G138" si="20">(C138*F138)</f>
+        <v>2556</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A139" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="B139" t="s">
+        <v>211</v>
+      </c>
+      <c r="C139" s="5"/>
+      <c r="D139" s="5">
+        <v>1</v>
+      </c>
+      <c r="E139" s="5">
+        <v>0</v>
+      </c>
+      <c r="F139">
+        <f t="shared" ref="F139:F141" si="21">(D139+E139)</f>
+        <v>1</v>
+      </c>
+      <c r="G139">
+        <f t="shared" ref="G139:G141" si="22">(C139*F139)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A140" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="B140" t="s">
+        <v>213</v>
+      </c>
+      <c r="C140" s="5"/>
+      <c r="D140" s="5">
+        <v>2</v>
+      </c>
+      <c r="E140" s="5">
+        <v>0</v>
+      </c>
+      <c r="F140">
+        <f t="shared" si="21"/>
+        <v>2</v>
+      </c>
+      <c r="G140">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A141" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="B129" t="s">
+      <c r="B141" t="s">
         <v>214</v>
       </c>
-      <c r="C129" s="5">
+      <c r="C141" s="5">
         <v>277</v>
       </c>
-      <c r="D129" s="5">
-        <v>1</v>
-      </c>
-      <c r="E129" s="5">
-        <v>0</v>
-      </c>
-      <c r="F129">
-        <f t="shared" si="15"/>
-        <v>1</v>
-      </c>
-      <c r="G129">
-        <f t="shared" si="16"/>
+      <c r="D141" s="5">
+        <v>1</v>
+      </c>
+      <c r="E141" s="5">
+        <v>0</v>
+      </c>
+      <c r="F141">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+      <c r="G141">
+        <f t="shared" si="22"/>
         <v>277</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A130" s="5" t="s">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A142" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="B130" t="s">
+      <c r="B142" t="s">
         <v>217</v>
       </c>
-      <c r="C130" s="5"/>
-      <c r="D130" s="5">
-        <v>1</v>
-      </c>
-      <c r="E130" s="5"/>
-      <c r="F130">
-        <f t="shared" ref="F130" si="17">(D130+E130)</f>
-        <v>1</v>
-      </c>
-      <c r="G130">
-        <f t="shared" ref="G130" si="18">(C130*F130)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A131" s="5"/>
-      <c r="C131" s="5"/>
-      <c r="D131" s="5"/>
-      <c r="E131" s="5"/>
-    </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A132" s="5"/>
-      <c r="C132" s="5"/>
-      <c r="D132" s="5"/>
-      <c r="E132" s="5"/>
-    </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A133" s="5"/>
-      <c r="C133" s="5"/>
-      <c r="D133" s="5"/>
-      <c r="E133" s="5"/>
-    </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
+      <c r="C142" s="5"/>
+      <c r="D142" s="5">
+        <v>1</v>
+      </c>
+      <c r="E142" s="5"/>
+      <c r="F142">
+        <f t="shared" ref="F142" si="23">(D142+E142)</f>
+        <v>1</v>
+      </c>
+      <c r="G142">
+        <f t="shared" ref="G142" si="24">(C142*F142)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A143" s="5"/>
+      <c r="C143" s="5"/>
+      <c r="D143" s="5"/>
+      <c r="E143" s="5"/>
+    </row>
+    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A144" s="5"/>
+      <c r="C144" s="5"/>
+      <c r="D144" s="5"/>
+      <c r="E144" s="5"/>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A145" s="5"/>
+      <c r="C145" s="5"/>
+      <c r="D145" s="5"/>
+      <c r="E145" s="5"/>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
         <v>178</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B68" r:id="rId1" display="http://swagelok.com/search/find_products_home.aspx?part=B-400-3TTM&amp;item=2cae453c-a275-4713-af4b-cd3f1469885c"/>
-    <hyperlink ref="B69" r:id="rId2" display="http://swagelok.com/search/find_products_home.aspx?part=SS-200-7-2&amp;item=20b6dcb5-5a04-42f1-9df7-a5d3fd3672c3"/>
-    <hyperlink ref="B70" r:id="rId3" display="http://swagelok.com/search/find_products_home.aspx?part=B-400-6-2&amp;item=20b6dcb5-5a04-42f1-9df7-a5d3fd3672c3"/>
-    <hyperlink ref="B71" r:id="rId4" display="http://swagelok.com/search/find_products_home.aspx?part=B-400-3&amp;item=2cae453c-a275-4713-af4b-cd3f1469885c"/>
-    <hyperlink ref="B72" r:id="rId5" display="http://swagelok.com/search/find_products_home.aspx?part=B-400-1-4BT&amp;item=20b6dcb5-5a04-42f1-9df7-a5d3fd3672c3"/>
-    <hyperlink ref="B73" r:id="rId6" display="http://swagelok.com/search/find_products_home.aspx?part=B-400-C&amp;item=0c0b2cd7-9ccc-4de3-9dd6-3c70e2fdde61"/>
-    <hyperlink ref="B77" r:id="rId7" display="http://swagelok.com/search/find_products_home.aspx?part=PFA-T2-030-100&amp;item=dc9ceee0-9c35-458d-a129-824c37ed3832"/>
-    <hyperlink ref="B82" r:id="rId8" display="http://swagelok.com/search/find_products_home.aspx?part=B-6-HC-1-4&amp;item=50b243b0-8a71-45ac-8579-0f1d438b0b8c"/>
-    <hyperlink ref="B81" r:id="rId9" display="http://swagelok.com/search/find_products_home.aspx?part=B-42XS4&amp;item=5c7e79e8-62ca-4c16-8b6e-0ba1530cbfd7"/>
-    <hyperlink ref="B83" r:id="rId10" display="http://swagelok.com/search/find_products_home.aspx?part=B-400-7-4&amp;item=20b6dcb5-5a04-42f1-9df7-a5d3fd3672c3"/>
-    <hyperlink ref="B84" r:id="rId11" display="http://swagelok.com/search/find_products_home.aspx?part=B-8-HC-1-4&amp;item=50b243b0-8a71-45ac-8579-0f1d438b0b8c"/>
-    <hyperlink ref="B85" r:id="rId12" display="http://swagelok.com/search/find_products_home.aspx?part=B-400-SET&amp;item=28a0d750-9482-4505-b72c-1b770fe8d100"/>
-    <hyperlink ref="B86" r:id="rId13" display="http://swagelok.com/search/find_products_home.aspx?part=B-200-SET&amp;item=28a0d750-9482-4505-b72c-1b770fe8d100"/>
-    <hyperlink ref="B92" r:id="rId14" display="http://www.mcmaster.com/"/>
-    <hyperlink ref="B93" r:id="rId15" display="http://www.mcmaster.com/"/>
-    <hyperlink ref="B94" r:id="rId16" display="http://www.mcmaster.com/"/>
-    <hyperlink ref="B95" r:id="rId17" display="http://www.mcmaster.com/"/>
-    <hyperlink ref="B97" r:id="rId18" display="http://www.mcmaster.com/"/>
-    <hyperlink ref="B98" r:id="rId19" display="http://www.mcmaster.com/"/>
-    <hyperlink ref="B99" r:id="rId20" display="http://www.mcmaster.com/"/>
-    <hyperlink ref="B100" r:id="rId21" display="http://www.mcmaster.com/"/>
-    <hyperlink ref="B101" r:id="rId22" display="http://www.mcmaster.com/"/>
-    <hyperlink ref="B102" r:id="rId23" display="http://www.mcmaster.com/"/>
-    <hyperlink ref="B103" r:id="rId24" display="http://www.mcmaster.com/"/>
-    <hyperlink ref="B104" r:id="rId25" display="http://www.mcmaster.com/"/>
-    <hyperlink ref="B105" r:id="rId26" display="http://www.mcmaster.com/"/>
-    <hyperlink ref="B106" r:id="rId27" display="http://www.mcmaster.com/"/>
+    <hyperlink ref="B71" r:id="rId1" display="http://swagelok.com/search/find_products_home.aspx?part=B-400-3TTM&amp;item=2cae453c-a275-4713-af4b-cd3f1469885c"/>
+    <hyperlink ref="B72" r:id="rId2" display="http://swagelok.com/search/find_products_home.aspx?part=SS-200-7-2&amp;item=20b6dcb5-5a04-42f1-9df7-a5d3fd3672c3"/>
+    <hyperlink ref="B75" r:id="rId3" display="http://swagelok.com/search/find_products_home.aspx?part=B-400-6-2&amp;item=20b6dcb5-5a04-42f1-9df7-a5d3fd3672c3"/>
+    <hyperlink ref="B76" r:id="rId4" display="http://swagelok.com/search/find_products_home.aspx?part=B-400-3&amp;item=2cae453c-a275-4713-af4b-cd3f1469885c"/>
+    <hyperlink ref="B77" r:id="rId5" display="http://swagelok.com/search/find_products_home.aspx?part=B-400-1-4BT&amp;item=20b6dcb5-5a04-42f1-9df7-a5d3fd3672c3"/>
+    <hyperlink ref="B78" r:id="rId6" display="http://swagelok.com/search/find_products_home.aspx?part=B-400-C&amp;item=0c0b2cd7-9ccc-4de3-9dd6-3c70e2fdde61"/>
+    <hyperlink ref="B82" r:id="rId7" display="http://swagelok.com/search/find_products_home.aspx?part=PFA-T2-030-100&amp;item=dc9ceee0-9c35-458d-a129-824c37ed3832"/>
+    <hyperlink ref="B87" r:id="rId8" display="http://swagelok.com/search/find_products_home.aspx?part=B-6-HC-1-4&amp;item=50b243b0-8a71-45ac-8579-0f1d438b0b8c"/>
+    <hyperlink ref="B86" r:id="rId9" display="http://swagelok.com/search/find_products_home.aspx?part=B-42XS4&amp;item=5c7e79e8-62ca-4c16-8b6e-0ba1530cbfd7"/>
+    <hyperlink ref="B88" r:id="rId10" display="http://swagelok.com/search/find_products_home.aspx?part=B-400-7-4&amp;item=20b6dcb5-5a04-42f1-9df7-a5d3fd3672c3"/>
+    <hyperlink ref="B89" r:id="rId11" display="http://swagelok.com/search/find_products_home.aspx?part=B-8-HC-1-4&amp;item=50b243b0-8a71-45ac-8579-0f1d438b0b8c"/>
+    <hyperlink ref="B90" r:id="rId12" display="http://swagelok.com/search/find_products_home.aspx?part=B-400-SET&amp;item=28a0d750-9482-4505-b72c-1b770fe8d100"/>
+    <hyperlink ref="B91" r:id="rId13" display="http://swagelok.com/search/find_products_home.aspx?part=B-200-SET&amp;item=28a0d750-9482-4505-b72c-1b770fe8d100"/>
+    <hyperlink ref="B97" r:id="rId14" display="http://www.mcmaster.com/"/>
+    <hyperlink ref="B98" r:id="rId15" display="http://www.mcmaster.com/"/>
+    <hyperlink ref="B99" r:id="rId16" display="http://www.mcmaster.com/"/>
+    <hyperlink ref="B100" r:id="rId17" display="http://www.mcmaster.com/"/>
+    <hyperlink ref="B102" r:id="rId18" display="http://www.mcmaster.com/"/>
+    <hyperlink ref="B103" r:id="rId19" display="http://www.mcmaster.com/"/>
+    <hyperlink ref="B104" r:id="rId20" display="http://www.mcmaster.com/"/>
+    <hyperlink ref="B107" r:id="rId21" display="http://www.mcmaster.com/"/>
+    <hyperlink ref="B108" r:id="rId22" display="http://www.mcmaster.com/"/>
+    <hyperlink ref="B109" r:id="rId23" display="http://www.mcmaster.com/"/>
+    <hyperlink ref="B110" r:id="rId24" display="http://www.mcmaster.com/"/>
+    <hyperlink ref="B111" r:id="rId25" display="http://www.mcmaster.com/"/>
+    <hyperlink ref="B112" r:id="rId26" display="http://www.mcmaster.com/"/>
+    <hyperlink ref="B113" r:id="rId27" display="http://www.mcmaster.com/"/>
+    <hyperlink ref="B105" r:id="rId28" location="9557K478" tooltip="Add this product to your current order" display="http://www.mcmaster.com/ - 9557K478"/>
+    <hyperlink ref="B106" r:id="rId29" location="9557K479" tooltip="Add this product to your current order" display="http://www.mcmaster.com/ - 9557K479"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId28"/>
+  <pageSetup orientation="portrait" r:id="rId30"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
fixed errors in lady gaga enclosure bill of materials and drawings.  added assembly diagrams
</commit_message>
<xml_diff>
--- a/Materials List/LADY GAGA V2 Materials.xlsx
+++ b/Materials List/LADY GAGA V2 Materials.xlsx
@@ -1140,8 +1140,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="H106" sqref="H106"/>
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="H120" sqref="H120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3392,7 +3392,7 @@
         <v>50</v>
       </c>
       <c r="G107">
-        <f t="shared" ref="G107:G114" si="17">(C107*F107)</f>
+        <f t="shared" ref="G107:G120" si="17">(C107*F107)</f>
         <v>19.5</v>
       </c>
     </row>
@@ -3630,7 +3630,7 @@
         <v>205</v>
       </c>
       <c r="C120">
-        <v>1702.97</v>
+        <v>1710.44</v>
       </c>
       <c r="D120">
         <v>1</v>
@@ -3642,7 +3642,7 @@
         <v>1</v>
       </c>
       <c r="G120">
-        <v>1702.97</v>
+        <v>1710.44</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
updated some drawings and created packet for meeting with jfrc
</commit_message>
<xml_diff>
--- a/Materials List/LADY GAGA V2 Materials.xlsx
+++ b/Materials List/LADY GAGA V2 Materials.xlsx
@@ -11,12 +11,15 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$G$154</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="249">
   <si>
     <t>Description</t>
   </si>
@@ -552,9 +555,6 @@
     <t>Need camera, acquisition board, computer, etc. for acquisition</t>
   </si>
   <si>
-    <t xml:space="preserve">Need enclosure with feedthroughs </t>
-  </si>
-  <si>
     <t>Custom electronics</t>
   </si>
   <si>
@@ -627,9 +627,6 @@
     <t>5805T11</t>
   </si>
   <si>
-    <t>Need to provide clean filtered air (charcoal filtered &amp; filtered at 35 microns or better) at 20 psi to mass flow controllers and, air to pneumatic clamp at adjustable pressure ~10 psi</t>
-  </si>
-  <si>
     <t>80/20</t>
   </si>
   <si>
@@ -754,6 +751,21 @@
   </si>
   <si>
     <t>9557K479</t>
+  </si>
+  <si>
+    <t>9277K38</t>
+  </si>
+  <si>
+    <t>Push-in Tapered Colored Rubber Plug Red, Fits 11/32" Large End ID, pack of 50</t>
+  </si>
+  <si>
+    <t>40025K26</t>
+  </si>
+  <si>
+    <t>Push-in Tapered Round Plug with Flange Std, Fits .31" ID Large End, 3/4" Height, Orange</t>
+  </si>
+  <si>
+    <t>Need to provide clean filtered air (charcoal filtered &amp; filtered at 35 microns or better) at 20 psi to mass flow controllers and air to pneumatic clamp at adjustable pressure ~10 psi</t>
   </si>
 </sst>
 </file>
@@ -1137,11 +1149,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:H154"/>
+  <sheetPr codeName="Sheet1">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:H156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="H120" sqref="H120"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H158" sqref="H158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1409,13 +1423,13 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B13" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C13" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -1430,13 +1444,13 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B14" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C14" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D14">
         <v>2</v>
@@ -1451,13 +1465,13 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B15" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C15" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D15">
         <v>2</v>
@@ -1470,12 +1484,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="21" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" ht="21" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>0</v>
       </c>
@@ -1498,7 +1512,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>41</v>
       </c>
@@ -1523,7 +1537,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>44</v>
       </c>
@@ -1548,7 +1562,7 @@
         <v>23.700000000000003</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>45</v>
       </c>
@@ -1573,7 +1587,7 @@
         <v>14.22</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>47</v>
       </c>
@@ -1598,7 +1612,7 @@
         <v>14.91</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>49</v>
       </c>
@@ -1623,7 +1637,7 @@
         <v>35.15</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>51</v>
       </c>
@@ -1648,7 +1662,7 @@
         <v>136.5</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>53</v>
       </c>
@@ -1673,7 +1687,7 @@
         <v>131.25</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>55</v>
       </c>
@@ -1698,7 +1712,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>57</v>
       </c>
@@ -1723,7 +1737,7 @@
         <v>11.3</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>59</v>
       </c>
@@ -1748,7 +1762,7 @@
         <v>106.1</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>61</v>
       </c>
@@ -1773,7 +1787,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>63</v>
       </c>
@@ -1798,22 +1812,28 @@
         <v>68</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H31">
+        <f>SUM(G19:G30)</f>
+        <v>1418.1299999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="21" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:8" ht="21" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>0</v>
       </c>
@@ -1836,7 +1856,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>68</v>
       </c>
@@ -1861,7 +1881,7 @@
         <v>1030.04</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>70</v>
       </c>
@@ -1886,7 +1906,7 @@
         <v>187.04</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>72</v>
       </c>
@@ -1911,12 +1931,12 @@
         <v>96.48</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B40" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C40">
         <v>85</v>
@@ -1936,7 +1956,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>74</v>
       </c>
@@ -1961,7 +1981,7 @@
         <v>85.19</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>75</v>
       </c>
@@ -1986,7 +2006,7 @@
         <v>23.82</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>77</v>
       </c>
@@ -2011,7 +2031,7 @@
         <v>11.91</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>79</v>
       </c>
@@ -2036,7 +2056,7 @@
         <v>170.72</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>81</v>
       </c>
@@ -2061,7 +2081,7 @@
         <v>13.3</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>83</v>
       </c>
@@ -2086,7 +2106,7 @@
         <v>21.1</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F47">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2095,8 +2115,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" ht="21" x14ac:dyDescent="0.35">
+      <c r="H47">
+        <f>SUM(G37:G46)</f>
+        <v>1724.6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="21" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="s">
         <v>85</v>
       </c>
@@ -2460,7 +2484,7 @@
         <v>145.28</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>108</v>
       </c>
@@ -2485,17 +2509,23 @@
         <v>106.81</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H66">
+        <f>SUM(G55:G65)</f>
+        <v>661.99</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="21" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:8" ht="21" x14ac:dyDescent="0.35">
       <c r="A69" s="2" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>0</v>
       </c>
@@ -2518,7 +2548,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>112</v>
       </c>
@@ -2543,7 +2573,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>114</v>
       </c>
@@ -2568,12 +2598,12 @@
         <v>28.200000000000003</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C73">
         <v>6.9</v>
@@ -2593,12 +2623,12 @@
         <v>41.400000000000006</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C74">
         <v>7.5</v>
@@ -2618,7 +2648,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>117</v>
       </c>
@@ -2643,7 +2673,7 @@
         <v>21.6</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>118</v>
       </c>
@@ -2668,7 +2698,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>124</v>
       </c>
@@ -2693,7 +2723,7 @@
         <v>8.6999999999999993</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>126</v>
       </c>
@@ -2718,7 +2748,7 @@
         <v>6.8</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>128</v>
       </c>
@@ -2743,7 +2773,7 @@
         <v>3.4</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>130</v>
       </c>
@@ -2768,7 +2798,7 @@
         <v>8.3999999999999986</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>132</v>
       </c>
@@ -2793,7 +2823,7 @@
         <v>17.600000000000001</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>135</v>
       </c>
@@ -2818,7 +2848,7 @@
         <v>96.4</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>136</v>
       </c>
@@ -2843,7 +2873,7 @@
         <v>129.9</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>138</v>
       </c>
@@ -2868,7 +2898,7 @@
         <v>46.4</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>140</v>
       </c>
@@ -2893,7 +2923,7 @@
         <v>34.9</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>144</v>
       </c>
@@ -2918,7 +2948,7 @@
         <v>44.1</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>143</v>
       </c>
@@ -2943,7 +2973,7 @@
         <v>6.8</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>146</v>
       </c>
@@ -2968,7 +2998,7 @@
         <v>6.8</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>149</v>
       </c>
@@ -2993,7 +3023,7 @@
         <v>5.2</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>150</v>
       </c>
@@ -3018,7 +3048,7 @@
         <v>7.4</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>153</v>
       </c>
@@ -3043,12 +3073,18 @@
         <v>7.6</v>
       </c>
     </row>
-    <row r="93" spans="1:7" ht="21" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H92">
+        <f>SUM(G71:G91)</f>
+        <v>647.59999999999991</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" ht="21" x14ac:dyDescent="0.35">
       <c r="A93" s="2" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>0</v>
       </c>
@@ -3071,7 +3107,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>154</v>
       </c>
@@ -3096,7 +3132,7 @@
         <v>33.28</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>155</v>
       </c>
@@ -3323,10 +3359,10 @@
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B105" s="6" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C105">
         <v>5.89</v>
@@ -3348,10 +3384,10 @@
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B106" s="6" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C106">
         <v>5.28</v>
@@ -3388,20 +3424,20 @@
         <v>0</v>
       </c>
       <c r="F107">
-        <f t="shared" ref="F107:F114" si="16">(D107+E107)</f>
+        <f t="shared" ref="F107:F116" si="16">(D107+E107)</f>
         <v>50</v>
       </c>
       <c r="G107">
-        <f t="shared" ref="G107:G120" si="17">(C107*F107)</f>
+        <f t="shared" ref="G107:G116" si="17">(C107*F107)</f>
         <v>19.5</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B108" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C108">
         <v>4.99</v>
@@ -3423,10 +3459,10 @@
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B109" s="6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C109">
         <v>5.01</v>
@@ -3448,10 +3484,10 @@
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
+        <v>192</v>
+      </c>
+      <c r="B110" s="6" t="s">
         <v>193</v>
-      </c>
-      <c r="B110" s="6" t="s">
-        <v>194</v>
       </c>
       <c r="C110">
         <v>5.65</v>
@@ -3473,10 +3509,10 @@
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
+        <v>194</v>
+      </c>
+      <c r="B111" s="6" t="s">
         <v>195</v>
-      </c>
-      <c r="B111" s="6" t="s">
-        <v>196</v>
       </c>
       <c r="C111">
         <v>7.08</v>
@@ -3498,10 +3534,10 @@
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
+        <v>196</v>
+      </c>
+      <c r="B112" s="6" t="s">
         <v>197</v>
-      </c>
-      <c r="B112" s="6" t="s">
-        <v>198</v>
       </c>
       <c r="C112">
         <v>2.87</v>
@@ -3523,10 +3559,10 @@
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
+        <v>198</v>
+      </c>
+      <c r="B113" s="6" t="s">
         <v>199</v>
-      </c>
-      <c r="B113" s="6" t="s">
-        <v>200</v>
       </c>
       <c r="C113">
         <v>3.13</v>
@@ -3548,10 +3584,10 @@
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
+        <v>200</v>
+      </c>
+      <c r="B114" t="s">
         <v>201</v>
-      </c>
-      <c r="B114" t="s">
-        <v>202</v>
       </c>
       <c r="C114">
         <v>13.94</v>
@@ -3571,460 +3607,533 @@
         <v>27.88</v>
       </c>
     </row>
-    <row r="117" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A117" s="2" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A118" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B118" s="1" t="s">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>245</v>
+      </c>
+      <c r="B115" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="C115">
+        <v>10.48</v>
+      </c>
+      <c r="D115">
+        <v>2</v>
+      </c>
+      <c r="E115">
+        <v>0</v>
+      </c>
+      <c r="F115">
+        <f t="shared" si="16"/>
+        <v>2</v>
+      </c>
+      <c r="G115">
+        <f t="shared" si="17"/>
+        <v>20.96</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>247</v>
+      </c>
+      <c r="B116" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="C116">
+        <v>11.91</v>
+      </c>
+      <c r="D116">
+        <v>0</v>
+      </c>
+      <c r="E116">
+        <v>2</v>
+      </c>
+      <c r="F116">
+        <f t="shared" si="16"/>
+        <v>2</v>
+      </c>
+      <c r="G116">
+        <f t="shared" si="17"/>
+        <v>23.82</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H117">
+        <f>SUM(G95:G116)</f>
+        <v>329.72999999999996</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A118" s="2" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A119" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B119" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C118" s="1" t="s">
+      <c r="C119" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D118" s="1" t="s">
+      <c r="D119" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E118" s="1" t="s">
+      <c r="E119" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F118" s="1" t="s">
+      <c r="F119" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G118" s="1" t="s">
+      <c r="G119" s="1" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
-        <v>206</v>
-      </c>
-      <c r="B119" s="7" t="s">
-        <v>205</v>
-      </c>
-      <c r="C119">
-        <v>381.45</v>
-      </c>
-      <c r="D119">
-        <v>1</v>
-      </c>
-      <c r="E119">
-        <v>0</v>
-      </c>
-      <c r="F119">
-        <v>1</v>
-      </c>
-      <c r="G119">
-        <v>381.45</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>221</v>
+        <v>204</v>
       </c>
       <c r="B120" s="7" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C120">
+        <v>381.45</v>
+      </c>
+      <c r="D120">
+        <v>1</v>
+      </c>
+      <c r="E120">
+        <v>0</v>
+      </c>
+      <c r="F120">
+        <v>1</v>
+      </c>
+      <c r="G120">
+        <v>381.45</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>219</v>
+      </c>
+      <c r="B121" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="C121">
         <v>1710.44</v>
       </c>
-      <c r="D120">
-        <v>1</v>
-      </c>
-      <c r="E120">
-        <v>0</v>
-      </c>
-      <c r="F120">
-        <v>1</v>
-      </c>
-      <c r="G120">
+      <c r="D121">
+        <v>1</v>
+      </c>
+      <c r="E121">
+        <v>0</v>
+      </c>
+      <c r="F121">
+        <v>1</v>
+      </c>
+      <c r="G121">
         <v>1710.44</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B121" s="6"/>
-    </row>
-    <row r="122" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A122" s="2" t="s">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B122" s="6"/>
+      <c r="H122">
+        <f>SUM(G120:G121)</f>
+        <v>2091.89</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A123" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A124" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D124" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E124" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F124" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G124" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A125" s="5" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A123" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B123" s="1" t="s">
+      <c r="B125" t="s">
+        <v>183</v>
+      </c>
+      <c r="C125" s="5">
+        <v>169</v>
+      </c>
+      <c r="D125" s="5">
+        <v>2</v>
+      </c>
+      <c r="E125" s="5">
+        <v>0</v>
+      </c>
+      <c r="F125">
+        <f t="shared" ref="F125" si="18">(D125+E125)</f>
+        <v>2</v>
+      </c>
+      <c r="G125">
+        <f t="shared" ref="G125" si="19">(C125*F125)</f>
+        <v>338</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A126" s="1"/>
+      <c r="B126" s="1"/>
+      <c r="C126" s="1"/>
+      <c r="D126" s="1"/>
+      <c r="E126" s="1"/>
+      <c r="F126" s="1"/>
+      <c r="G126" s="1"/>
+      <c r="H126">
+        <f>SUM(G125)</f>
+        <v>338</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A127" s="2" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A128" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B128" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C123" s="1" t="s">
+      <c r="C128" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D123" s="1" t="s">
+      <c r="D128" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E123" s="1" t="s">
+      <c r="E128" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F123" s="1" t="s">
+      <c r="F128" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G123" s="1" t="s">
+      <c r="G128" s="1" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A124" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="B124" t="s">
-        <v>184</v>
-      </c>
-      <c r="C124" s="5">
-        <v>169</v>
-      </c>
-      <c r="D124" s="5">
-        <v>2</v>
-      </c>
-      <c r="E124" s="5">
-        <v>0</v>
-      </c>
-      <c r="F124">
-        <f t="shared" ref="F124" si="18">(D124+E124)</f>
-        <v>2</v>
-      </c>
-      <c r="G124">
-        <f t="shared" ref="G124" si="19">(C124*F124)</f>
-        <v>338</v>
-      </c>
-    </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A125" s="1"/>
-      <c r="B125" s="1"/>
-      <c r="C125" s="1"/>
-      <c r="D125" s="1"/>
-      <c r="E125" s="1"/>
-      <c r="F125" s="1"/>
-      <c r="G125" s="1"/>
-    </row>
-    <row r="126" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A126" s="2" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A127" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B127" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C127" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D127" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E127" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F127" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G127" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A128" s="5" t="s">
-        <v>233</v>
-      </c>
-      <c r="B128" t="s">
-        <v>232</v>
-      </c>
-      <c r="C128" s="5">
-        <v>540</v>
-      </c>
-      <c r="D128" s="5">
-        <v>2</v>
-      </c>
-      <c r="E128" s="5">
-        <v>0</v>
-      </c>
-      <c r="F128">
-        <f>(D128+E128)</f>
-        <v>2</v>
-      </c>
-      <c r="G128">
-        <f>(C128*F128)</f>
-        <v>1080</v>
-      </c>
-      <c r="H128" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" s="5" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B129" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="C129" s="5">
-        <v>675</v>
+        <v>540</v>
       </c>
       <c r="D129" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E129" s="5">
         <v>0</v>
       </c>
       <c r="F129">
         <f>(D129+E129)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G129">
         <f>(C129*F129)</f>
+        <v>1080</v>
+      </c>
+      <c r="H129" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A130" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="B130" t="s">
+        <v>233</v>
+      </c>
+      <c r="C130" s="5">
         <v>675</v>
       </c>
-      <c r="H129" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A130" s="1"/>
-      <c r="B130" s="1"/>
-      <c r="C130" s="1"/>
-      <c r="D130" s="1"/>
-      <c r="E130" s="1"/>
-      <c r="F130" s="1"/>
-      <c r="G130" s="1"/>
-    </row>
-    <row r="131" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A131" s="2" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
-        <v>180</v>
-      </c>
-      <c r="B133" t="s">
-        <v>218</v>
+      <c r="D130" s="5">
+        <v>1</v>
+      </c>
+      <c r="E130" s="5">
+        <v>0</v>
+      </c>
+      <c r="F130">
+        <f>(D130+E130)</f>
+        <v>1</v>
+      </c>
+      <c r="G130">
+        <f>(C130*F130)</f>
+        <v>675</v>
+      </c>
+      <c r="H130" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A131" s="1"/>
+      <c r="B131" s="1"/>
+      <c r="C131" s="1"/>
+      <c r="D131" s="1"/>
+      <c r="E131" s="1"/>
+      <c r="F131" s="1"/>
+      <c r="G131" s="1"/>
+      <c r="H131">
+        <f>SUM(G129:G130)</f>
+        <v>1755</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A132" s="2" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B134" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="136" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A136" s="2" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A137" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B137" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>180</v>
+      </c>
+      <c r="B135" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A137" s="2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A138" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B138" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C137" s="1" t="s">
+      <c r="C138" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D137" s="1" t="s">
+      <c r="D138" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E137" s="1" t="s">
+      <c r="E138" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F137" s="1" t="s">
+      <c r="F138" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G137" s="1" t="s">
+      <c r="G138" s="1" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A138" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="B138" t="s">
-        <v>208</v>
-      </c>
-      <c r="C138" s="5">
-        <v>852</v>
-      </c>
-      <c r="D138" s="5">
-        <v>3</v>
-      </c>
-      <c r="E138" s="5">
-        <v>0</v>
-      </c>
-      <c r="F138">
-        <f>(D138+E138)</f>
-        <v>3</v>
-      </c>
-      <c r="G138">
-        <f t="shared" ref="G138" si="20">(C138*F138)</f>
-        <v>2556</v>
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139" s="5" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B139" t="s">
-        <v>211</v>
-      </c>
-      <c r="C139" s="5"/>
+        <v>206</v>
+      </c>
+      <c r="C139" s="5">
+        <v>852</v>
+      </c>
       <c r="D139" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E139" s="5">
         <v>0</v>
       </c>
       <c r="F139">
-        <f t="shared" ref="F139:F141" si="21">(D139+E139)</f>
-        <v>1</v>
+        <f>(D139+E139)</f>
+        <v>3</v>
       </c>
       <c r="G139">
-        <f t="shared" ref="G139:G141" si="22">(C139*F139)</f>
-        <v>0</v>
+        <f t="shared" ref="G139" si="20">(C139*F139)</f>
+        <v>2556</v>
       </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140" s="5" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="B140" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C140" s="5"/>
       <c r="D140" s="5">
+        <v>1</v>
+      </c>
+      <c r="E140" s="5">
+        <v>0</v>
+      </c>
+      <c r="F140">
+        <f t="shared" ref="F140:F142" si="21">(D140+E140)</f>
+        <v>1</v>
+      </c>
+      <c r="G140">
+        <f t="shared" ref="G140:G142" si="22">(C140*F140)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A141" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="B141" t="s">
+        <v>211</v>
+      </c>
+      <c r="C141" s="5"/>
+      <c r="D141" s="5">
         <v>2</v>
       </c>
-      <c r="E140" s="5">
-        <v>0</v>
-      </c>
-      <c r="F140">
+      <c r="E141" s="5">
+        <v>0</v>
+      </c>
+      <c r="F141">
         <f t="shared" si="21"/>
         <v>2</v>
       </c>
-      <c r="G140">
-        <f t="shared" si="22"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A141" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="B141" t="s">
-        <v>214</v>
-      </c>
-      <c r="C141" s="5">
-        <v>277</v>
-      </c>
-      <c r="D141" s="5">
-        <v>1</v>
-      </c>
-      <c r="E141" s="5">
-        <v>0</v>
-      </c>
-      <c r="F141">
-        <f t="shared" si="21"/>
-        <v>1</v>
-      </c>
       <c r="G141">
         <f t="shared" si="22"/>
-        <v>277</v>
+        <v>0</v>
       </c>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142" s="5" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B142" t="s">
-        <v>217</v>
-      </c>
-      <c r="C142" s="5"/>
+        <v>212</v>
+      </c>
+      <c r="C142" s="5">
+        <v>277</v>
+      </c>
       <c r="D142" s="5">
         <v>1</v>
       </c>
-      <c r="E142" s="5"/>
+      <c r="E142" s="5">
+        <v>0</v>
+      </c>
       <c r="F142">
-        <f t="shared" ref="F142" si="23">(D142+E142)</f>
+        <f t="shared" si="21"/>
         <v>1</v>
       </c>
       <c r="G142">
-        <f t="shared" ref="G142" si="24">(C142*F142)</f>
-        <v>0</v>
+        <f t="shared" si="22"/>
+        <v>277</v>
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A143" s="5"/>
+      <c r="A143" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="B143" t="s">
+        <v>215</v>
+      </c>
       <c r="C143" s="5"/>
-      <c r="D143" s="5"/>
+      <c r="D143" s="5">
+        <v>1</v>
+      </c>
       <c r="E143" s="5"/>
+      <c r="F143">
+        <f t="shared" ref="F143" si="23">(D143+E143)</f>
+        <v>1</v>
+      </c>
+      <c r="G143">
+        <f t="shared" ref="G143" si="24">(C143*F143)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A144" s="5"/>
       <c r="C144" s="5"/>
       <c r="D144" s="5"/>
       <c r="E144" s="5"/>
-    </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H144">
+        <f>SUM(G139:G142)</f>
+        <v>2833</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145" s="5"/>
       <c r="C145" s="5"/>
       <c r="D145" s="5"/>
       <c r="E145" s="5"/>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A146" t="s">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A146" s="5"/>
+      <c r="C146" s="5"/>
+      <c r="D146" s="5"/>
+      <c r="E146" s="5"/>
+    </row>
+    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A147" t="s">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A148" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A149" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A151" t="s">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A152" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A154" t="s">
-        <v>178</v>
+    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H156">
+        <f>SUM(H144,H131,H126,H122,H117,H92,H66,H47,H31)</f>
+        <v>11799.939999999999</v>
       </c>
     </row>
   </sheetData>
@@ -4058,9 +4167,11 @@
     <hyperlink ref="B113" r:id="rId27" display="http://www.mcmaster.com/"/>
     <hyperlink ref="B105" r:id="rId28" location="9557K478" tooltip="Add this product to your current order" display="http://www.mcmaster.com/ - 9557K478"/>
     <hyperlink ref="B106" r:id="rId29" location="9557K479" tooltip="Add this product to your current order" display="http://www.mcmaster.com/ - 9557K479"/>
+    <hyperlink ref="B115" r:id="rId30" location="9277K38" tooltip="Add this product to your current order" display="http://www.mcmaster.com/ - 9277K38"/>
+    <hyperlink ref="B116" r:id="rId31" location="40025K26" tooltip="Add this product to your current order" display="http://www.mcmaster.com/ - 40025K26"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId30"/>
+  <pageSetup scale="57" fitToHeight="0" orientation="portrait" r:id="rId32"/>
 </worksheet>
 </file>
 

</xml_diff>